<commit_message>
First cut of nested dynamic lists
</commit_message>
<xml_diff>
--- a/test/resources/definitionsFiles/fe-automation-definition-v03.xlsx
+++ b/test/resources/definitionsFiles/fe-automation-definition-v03.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dev/Documents/Definition Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohammedanaskhatri/project/ccd-case-management-web/test/resources/definitionsFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C03B15-2E2B-B642-8670-12D7B70880B4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86BA22BF-2A59-7747-B7D4-B01C965D3C9B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
     <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId18"/>
     <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1704" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1729" uniqueCount="423">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1365,17 +1365,44 @@
   </si>
   <si>
     <t>Case Reference</t>
+  </si>
+  <si>
+    <t>Reference Collecrions</t>
+  </si>
+  <si>
+    <t>MaxLength: 1000</t>
+  </si>
+  <si>
+    <t>DisplayContextParameter</t>
+  </si>
+  <si>
+    <t>#TABLE(Title, FirstName, MiddleName)</t>
+  </si>
+  <si>
+    <t>ReferenceCollectionTab</t>
+  </si>
+  <si>
+    <t>referenceCollection</t>
+  </si>
+  <si>
+    <t>Reference Collection</t>
+  </si>
+  <si>
+    <t>SingleFormPage1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="&quot;DD/&quot;mm&quot;/YYYY&quot;"/>
     <numFmt numFmtId="165" formatCode="&quot;D/&quot;m&quot;/YY&quot;"/>
+    <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="167" formatCode="dd\/mm\/yyyy"/>
+    <numFmt numFmtId="168" formatCode="d\/m\/yy"/>
   </numFmts>
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -1556,6 +1583,25 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1583,7 +1629,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1662,13 +1708,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFAAAAAA"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1753,6 +1808,25 @@
     <xf numFmtId="164" fontId="29" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="29" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="23" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="13" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="32" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="23" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="23" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="166" fontId="32" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="32" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -2918,7 +2992,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3016,17 +3090,17 @@
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
     </row>
-    <row r="5" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
+    <row r="5" spans="1:10" s="84" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="89"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
     </row>
     <row r="6" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="7"/>
@@ -3099,10 +3173,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="A23" sqref="A23:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3518,23 +3592,23 @@
       <c r="A23" s="29"/>
       <c r="B23" s="29"/>
       <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
+      <c r="D23" s="8"/>
       <c r="E23" s="19"/>
       <c r="F23" s="28"/>
     </row>
     <row r="24" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="29"/>
       <c r="B24" s="29"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="59"/>
       <c r="F24" s="28"/>
     </row>
     <row r="25" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="29"/>
       <c r="B25" s="29"/>
       <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
+      <c r="D25" s="58"/>
       <c r="E25" s="19"/>
       <c r="F25" s="28"/>
     </row>
@@ -3542,49 +3616,25 @@
       <c r="A26" s="29"/>
       <c r="B26" s="29"/>
       <c r="C26" s="19"/>
-      <c r="D26" s="8"/>
+      <c r="D26" s="58"/>
       <c r="E26" s="19"/>
       <c r="F26" s="28"/>
     </row>
     <row r="27" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="29"/>
       <c r="B27" s="29"/>
-      <c r="C27" s="59"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="59"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
       <c r="F27" s="28"/>
     </row>
     <row r="28" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="29"/>
       <c r="B28" s="29"/>
       <c r="C28" s="19"/>
-      <c r="D28" s="58"/>
+      <c r="D28" s="19"/>
       <c r="E28" s="19"/>
       <c r="F28" s="28"/>
-    </row>
-    <row r="29" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="29"/>
-      <c r="B29" s="29"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="58"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="28"/>
-    </row>
-    <row r="30" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="29"/>
-      <c r="B30" s="29"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="28"/>
-    </row>
-    <row r="31" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="29"/>
-      <c r="B31" s="29"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
@@ -3600,7 +3650,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A11" sqref="A11:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3861,7 +3911,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="A11" sqref="A11:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4071,7 +4121,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4342,6 +4392,45 @@
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
     </row>
+    <row r="12" spans="1:11" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="10"/>
+      <c r="B12" s="90"/>
+      <c r="C12" s="80"/>
+      <c r="D12" s="80"/>
+      <c r="E12" s="82"/>
+      <c r="F12" s="91"/>
+      <c r="G12" s="91"/>
+      <c r="H12" s="91"/>
+      <c r="I12" s="91"/>
+      <c r="J12" s="91"/>
+      <c r="K12" s="91"/>
+    </row>
+    <row r="13" spans="1:11" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="10"/>
+      <c r="B13" s="91"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="80"/>
+      <c r="E13" s="82"/>
+      <c r="F13" s="91"/>
+      <c r="G13" s="91"/>
+      <c r="H13" s="91"/>
+      <c r="I13" s="91"/>
+      <c r="J13" s="91"/>
+      <c r="K13" s="91"/>
+    </row>
+    <row r="14" spans="1:11" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="10"/>
+      <c r="B14" s="91"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="82"/>
+      <c r="F14" s="91"/>
+      <c r="G14" s="91"/>
+      <c r="H14" s="91"/>
+      <c r="I14" s="91"/>
+      <c r="J14" s="91"/>
+      <c r="K14" s="91"/>
+    </row>
     <row r="22" spans="2:2" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="8"/>
     </row>
@@ -4356,10 +4445,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4482,21 +4571,8 @@
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
     </row>
-    <row r="6" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-    </row>
-    <row r="19" spans="5:5" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E19" s="43"/>
+    <row r="18" spans="5:5" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E18" s="43"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4515,7 +4591,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4708,10 +4784,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:XFD38"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4796,28 +4872,28 @@
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" s="84" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="10">
         <v>42736</v>
       </c>
-      <c r="B4" s="10"/>
+      <c r="B4" s="85"/>
       <c r="C4" s="8" t="s">
         <v>399</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>66</v>
+      <c r="D4" s="83" t="s">
+        <v>420</v>
       </c>
       <c r="E4" t="s">
         <v>271</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="86" t="s">
         <v>244</v>
       </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="87"/>
+      <c r="K4" s="88"/>
     </row>
     <row r="5" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="10">
@@ -4828,7 +4904,7 @@
         <v>399</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E5" t="s">
         <v>271</v>
@@ -4851,7 +4927,7 @@
         <v>399</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E6" t="s">
         <v>271</v>
@@ -4874,7 +4950,7 @@
         <v>399</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E7" t="s">
         <v>271</v>
@@ -4897,7 +4973,7 @@
         <v>399</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E8" t="s">
         <v>271</v>
@@ -4920,7 +4996,7 @@
         <v>399</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E9" t="s">
         <v>271</v>
@@ -4943,7 +5019,7 @@
         <v>399</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E10" t="s">
         <v>271</v>
@@ -4966,7 +5042,7 @@
         <v>399</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="E11" t="s">
         <v>271</v>
@@ -4989,7 +5065,7 @@
         <v>399</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="E12" t="s">
         <v>271</v>
@@ -5012,7 +5088,7 @@
         <v>399</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E13" t="s">
         <v>271</v>
@@ -5030,12 +5106,12 @@
       <c r="A14" s="10">
         <v>42736</v>
       </c>
-      <c r="B14" s="7"/>
+      <c r="B14" s="10"/>
       <c r="C14" s="8" t="s">
         <v>399</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="E14" t="s">
         <v>271</v>
@@ -5043,7 +5119,7 @@
       <c r="F14" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="G14" s="7"/>
+      <c r="G14" s="8"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
@@ -5058,7 +5134,7 @@
         <v>399</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E15" t="s">
         <v>271</v>
@@ -5072,7 +5148,7 @@
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
     </row>
-    <row r="16" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="10">
         <v>42736</v>
       </c>
@@ -5081,7 +5157,7 @@
         <v>399</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>270</v>
+        <v>88</v>
       </c>
       <c r="E16" t="s">
         <v>271</v>
@@ -5101,10 +5177,10 @@
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="8" t="s">
-        <v>275</v>
+        <v>399</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="E17" t="s">
         <v>271</v>
@@ -5118,15 +5194,16 @@
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
     </row>
-    <row r="18" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="10">
         <v>42736</v>
       </c>
+      <c r="B18" s="7"/>
       <c r="C18" s="8" t="s">
         <v>275</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E18" t="s">
         <v>271</v>
@@ -5134,17 +5211,21 @@
       <c r="F18" s="8" t="s">
         <v>244</v>
       </c>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
     </row>
     <row r="19" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="10">
         <v>42736</v>
       </c>
-      <c r="B19" s="43"/>
       <c r="C19" s="8" t="s">
         <v>275</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E19" t="s">
         <v>271</v>
@@ -5152,21 +5233,17 @@
       <c r="F19" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
-      <c r="K19" s="43"/>
     </row>
     <row r="20" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="10">
         <v>42736</v>
       </c>
+      <c r="B20" s="43"/>
       <c r="C20" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="D20" s="58" t="s">
-        <v>369</v>
+      <c r="D20" s="8" t="s">
+        <v>278</v>
       </c>
       <c r="E20" t="s">
         <v>271</v>
@@ -5174,17 +5251,21 @@
       <c r="F20" s="8" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="43"/>
+      <c r="K20" s="43"/>
+    </row>
+    <row r="21" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="10">
         <v>42736</v>
       </c>
-      <c r="B21" s="43"/>
-      <c r="C21" s="62" t="s">
-        <v>285</v>
+      <c r="C21" s="8" t="s">
+        <v>275</v>
       </c>
       <c r="D21" s="58" t="s">
-        <v>298</v>
+        <v>369</v>
       </c>
       <c r="E21" t="s">
         <v>271</v>
@@ -5192,11 +5273,6 @@
       <c r="F21" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="G21" s="43"/>
-      <c r="H21" s="43"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="43"/>
-      <c r="K21" s="43"/>
     </row>
     <row r="22" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10">
@@ -5207,7 +5283,7 @@
         <v>285</v>
       </c>
       <c r="D22" s="58" t="s">
-        <v>316</v>
+        <v>298</v>
       </c>
       <c r="E22" t="s">
         <v>271</v>
@@ -5230,7 +5306,7 @@
         <v>285</v>
       </c>
       <c r="D23" s="58" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="E23" t="s">
         <v>271</v>
@@ -5244,16 +5320,16 @@
       <c r="J23" s="43"/>
       <c r="K23" s="43"/>
     </row>
-    <row r="24" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="10">
         <v>42736</v>
       </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="58" t="s">
-        <v>332</v>
+      <c r="B24" s="43"/>
+      <c r="C24" s="62" t="s">
+        <v>285</v>
       </c>
       <c r="D24" s="58" t="s">
-        <v>335</v>
+        <v>313</v>
       </c>
       <c r="E24" t="s">
         <v>271</v>
@@ -5261,11 +5337,11 @@
       <c r="F24" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="G24" s="8"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
+      <c r="J24" s="43"/>
+      <c r="K24" s="43"/>
     </row>
     <row r="25" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="10">
@@ -5276,7 +5352,7 @@
         <v>332</v>
       </c>
       <c r="D25" s="58" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E25" t="s">
         <v>271</v>
@@ -5299,7 +5375,7 @@
         <v>332</v>
       </c>
       <c r="D26" s="58" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E26" t="s">
         <v>271</v>
@@ -5322,7 +5398,7 @@
         <v>332</v>
       </c>
       <c r="D27" s="58" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="E27" t="s">
         <v>271</v>
@@ -5345,7 +5421,7 @@
         <v>332</v>
       </c>
       <c r="D28" s="58" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E28" t="s">
         <v>271</v>
@@ -5368,7 +5444,7 @@
         <v>332</v>
       </c>
       <c r="D29" s="58" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E29" t="s">
         <v>271</v>
@@ -5391,7 +5467,7 @@
         <v>332</v>
       </c>
       <c r="D30" s="58" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E30" t="s">
         <v>271</v>
@@ -5414,7 +5490,7 @@
         <v>332</v>
       </c>
       <c r="D31" s="58" t="s">
-        <v>367</v>
+        <v>341</v>
       </c>
       <c r="E31" t="s">
         <v>271</v>
@@ -5437,7 +5513,7 @@
         <v>332</v>
       </c>
       <c r="D32" s="58" t="s">
-        <v>351</v>
+        <v>367</v>
       </c>
       <c r="E32" t="s">
         <v>271</v>
@@ -5460,7 +5536,7 @@
         <v>332</v>
       </c>
       <c r="D33" s="58" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="E33" t="s">
         <v>271</v>
@@ -5480,10 +5556,10 @@
       </c>
       <c r="B34" s="10"/>
       <c r="C34" s="58" t="s">
-        <v>376</v>
+        <v>332</v>
       </c>
       <c r="D34" s="58" t="s">
-        <v>335</v>
+        <v>357</v>
       </c>
       <c r="E34" t="s">
         <v>271</v>
@@ -5506,7 +5582,7 @@
         <v>376</v>
       </c>
       <c r="D35" s="58" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E35" t="s">
         <v>271</v>
@@ -5529,7 +5605,7 @@
         <v>376</v>
       </c>
       <c r="D36" s="58" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E36" t="s">
         <v>271</v>
@@ -5552,7 +5628,7 @@
         <v>376</v>
       </c>
       <c r="D37" s="58" t="s">
-        <v>390</v>
+        <v>339</v>
       </c>
       <c r="E37" t="s">
         <v>271</v>
@@ -5571,11 +5647,11 @@
         <v>42736</v>
       </c>
       <c r="B38" s="10"/>
-      <c r="C38" s="8" t="s">
-        <v>395</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>66</v>
+      <c r="C38" s="58" t="s">
+        <v>376</v>
+      </c>
+      <c r="D38" s="58" t="s">
+        <v>390</v>
       </c>
       <c r="E38" t="s">
         <v>271</v>
@@ -5595,7 +5671,7 @@
       </c>
       <c r="B39" s="10"/>
       <c r="C39" s="8" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>66</v>
@@ -5620,8 +5696,8 @@
       <c r="C40" s="8" t="s">
         <v>400</v>
       </c>
-      <c r="D40" s="58" t="s">
-        <v>336</v>
+      <c r="D40" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="E40" t="s">
         <v>271</v>
@@ -5644,7 +5720,7 @@
         <v>400</v>
       </c>
       <c r="D41" s="58" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E41" t="s">
         <v>271</v>
@@ -5657,6 +5733,29 @@
       <c r="I41" s="7"/>
       <c r="J41" s="7"/>
       <c r="K41" s="7"/>
+    </row>
+    <row r="42" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B42" s="10"/>
+      <c r="C42" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="D42" s="58" t="s">
+        <v>339</v>
+      </c>
+      <c r="E42" t="s">
+        <v>271</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="G42" s="8"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
@@ -5788,7 +5887,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6183,10 +6282,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6295,12 +6394,22 @@
       <c r="K4" s="7"/>
     </row>
     <row r="5" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="10"/>
+      <c r="A5" s="10">
+        <v>42736</v>
+      </c>
       <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="C5" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>268</v>
+      </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
@@ -6308,42 +6417,42 @@
       <c r="K5" s="7"/>
     </row>
     <row r="6" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="10">
-        <v>42736</v>
-      </c>
+      <c r="A6" s="40"/>
       <c r="B6" s="7"/>
-      <c r="C6" s="8" t="s">
-        <v>399</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>262</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>268</v>
-      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
     </row>
-    <row r="7" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="40"/>
+    <row r="7" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="10">
+        <v>42736</v>
+      </c>
       <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
+      <c r="C7" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="E7" s="55" t="s">
+        <v>271</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>244</v>
+      </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="10">
         <v>42736</v>
       </c>
@@ -6351,8 +6460,8 @@
       <c r="C8" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>166</v>
+      <c r="D8" s="58" t="s">
+        <v>330</v>
       </c>
       <c r="E8" s="55" t="s">
         <v>271</v>
@@ -6371,11 +6480,11 @@
         <v>42736</v>
       </c>
       <c r="B9" s="7"/>
-      <c r="C9" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="D9" s="58" t="s">
-        <v>330</v>
+      <c r="C9" s="58" t="s">
+        <v>285</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>166</v>
       </c>
       <c r="E9" s="55" t="s">
         <v>271</v>
@@ -6395,7 +6504,7 @@
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="58" t="s">
-        <v>285</v>
+        <v>332</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>166</v>
@@ -6418,9 +6527,9 @@
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="58" t="s">
-        <v>332</v>
-      </c>
-      <c r="D11" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="D11" s="67" t="s">
         <v>166</v>
       </c>
       <c r="E11" s="55" t="s">
@@ -6443,8 +6552,8 @@
       <c r="C12" s="58" t="s">
         <v>376</v>
       </c>
-      <c r="D12" s="67" t="s">
-        <v>166</v>
+      <c r="D12" s="68" t="s">
+        <v>377</v>
       </c>
       <c r="E12" s="55" t="s">
         <v>271</v>
@@ -6467,7 +6576,7 @@
         <v>376</v>
       </c>
       <c r="D13" s="68" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="E13" s="55" t="s">
         <v>271</v>
@@ -6486,11 +6595,11 @@
         <v>42736</v>
       </c>
       <c r="B14" s="7"/>
-      <c r="C14" s="58" t="s">
-        <v>376</v>
-      </c>
-      <c r="D14" s="68" t="s">
-        <v>378</v>
+      <c r="C14" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>166</v>
       </c>
       <c r="E14" s="55" t="s">
         <v>271</v>
@@ -6510,7 +6619,7 @@
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="8" t="s">
-        <v>395</v>
+        <v>400</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>166</v>
@@ -6526,29 +6635,6 @@
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
-    </row>
-    <row r="16" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="8" t="s">
-        <v>400</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="E16" s="55" t="s">
-        <v>271</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
@@ -6563,8 +6649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6886,10 +6972,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:IV41"/>
+  <dimension ref="A1:IV42"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7638,7 +7724,7 @@
     </row>
     <row r="16" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="10">
-        <v>42736</v>
+        <v>42737</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="8" t="s">
@@ -7671,23 +7757,25 @@
     </row>
     <row r="17" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="10">
-        <v>42736</v>
+        <v>42738</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>47</v>
+        <v>399</v>
+      </c>
+      <c r="D17" s="81" t="s">
+        <v>420</v>
+      </c>
+      <c r="E17" s="81" t="s">
+        <v>421</v>
       </c>
       <c r="F17" s="7"/>
-      <c r="G17" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="H17" s="8"/>
+      <c r="G17" s="80" t="s">
+        <v>64</v>
+      </c>
+      <c r="H17" s="81" t="s">
+        <v>65</v>
+      </c>
       <c r="I17" s="7"/>
       <c r="J17" s="8" t="s">
         <v>27</v>
@@ -7939,7 +8027,7 @@
       <c r="IU17" s="43"/>
       <c r="IV17" s="43"/>
     </row>
-    <row r="18" spans="1:256" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="10">
         <v>42736</v>
       </c>
@@ -7948,10 +8036,10 @@
         <v>275</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>109</v>
+        <v>47</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="8" t="s">
@@ -8217,11 +8305,11 @@
       <c r="C19" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="D19" s="57" t="s">
-        <v>278</v>
+      <c r="D19" s="8" t="s">
+        <v>277</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>50</v>
+        <v>109</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="8" t="s">
@@ -8487,15 +8575,15 @@
       <c r="C20" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="D20" s="58" t="s">
-        <v>369</v>
-      </c>
-      <c r="E20" s="58" t="s">
-        <v>369</v>
+      <c r="D20" s="57" t="s">
+        <v>278</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>50</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="8" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="H20" s="8"/>
       <c r="I20" s="7"/>
@@ -8755,17 +8843,17 @@
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="8" t="s">
-        <v>285</v>
-      </c>
-      <c r="D21" s="57" t="s">
-        <v>313</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>314</v>
+        <v>275</v>
+      </c>
+      <c r="D21" s="58" t="s">
+        <v>369</v>
+      </c>
+      <c r="E21" s="58" t="s">
+        <v>369</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="8" t="s">
-        <v>288</v>
+        <v>56</v>
       </c>
       <c r="H21" s="8"/>
       <c r="I21" s="7"/>
@@ -9027,15 +9115,15 @@
       <c r="C22" s="8" t="s">
         <v>285</v>
       </c>
-      <c r="D22" s="60" t="s">
-        <v>316</v>
-      </c>
-      <c r="E22" s="58" t="s">
-        <v>317</v>
+      <c r="D22" s="57" t="s">
+        <v>313</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>314</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="8" t="s">
-        <v>52</v>
+        <v>288</v>
       </c>
       <c r="H22" s="8"/>
       <c r="I22" s="7"/>
@@ -9298,18 +9386,16 @@
         <v>285</v>
       </c>
       <c r="D23" s="60" t="s">
-        <v>298</v>
+        <v>316</v>
       </c>
       <c r="E23" s="58" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="F23" s="7"/>
-      <c r="G23" s="58" t="s">
-        <v>64</v>
-      </c>
-      <c r="H23" s="58" t="s">
-        <v>299</v>
-      </c>
+      <c r="G23" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H23" s="8"/>
       <c r="I23" s="7"/>
       <c r="J23" s="8" t="s">
         <v>27</v>
@@ -9561,25 +9647,27 @@
       <c r="IU23" s="43"/>
       <c r="IV23" s="43"/>
     </row>
-    <row r="24" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:256" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="10">
         <v>42736</v>
       </c>
       <c r="B24" s="10"/>
-      <c r="C24" s="58" t="s">
-        <v>332</v>
-      </c>
-      <c r="D24" s="58" t="s">
-        <v>335</v>
+      <c r="C24" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="D24" s="60" t="s">
+        <v>298</v>
       </c>
       <c r="E24" s="58" t="s">
-        <v>333</v>
-      </c>
-      <c r="F24" s="63"/>
-      <c r="G24" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="H24" s="7"/>
+        <v>320</v>
+      </c>
+      <c r="F24" s="7"/>
+      <c r="G24" s="58" t="s">
+        <v>64</v>
+      </c>
+      <c r="H24" s="58" t="s">
+        <v>299</v>
+      </c>
       <c r="I24" s="7"/>
       <c r="J24" s="8" t="s">
         <v>27</v>
@@ -9840,12 +9928,12 @@
         <v>332</v>
       </c>
       <c r="D25" s="58" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E25" s="58" t="s">
-        <v>334</v>
-      </c>
-      <c r="F25" s="7"/>
+        <v>333</v>
+      </c>
+      <c r="F25" s="63"/>
       <c r="G25" s="8" t="s">
         <v>48</v>
       </c>
@@ -10110,10 +10198,10 @@
         <v>332</v>
       </c>
       <c r="D26" s="58" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E26" s="58" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="8" t="s">
@@ -10380,10 +10468,10 @@
         <v>332</v>
       </c>
       <c r="D27" s="58" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="E27" s="58" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="8" t="s">
@@ -10650,10 +10738,10 @@
         <v>332</v>
       </c>
       <c r="D28" s="58" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E28" s="58" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="8" t="s">
@@ -10920,10 +11008,10 @@
         <v>332</v>
       </c>
       <c r="D29" s="58" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E29" s="58" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="8" t="s">
@@ -11190,10 +11278,10 @@
         <v>332</v>
       </c>
       <c r="D30" s="58" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E30" s="58" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="8" t="s">
@@ -11460,14 +11548,12 @@
         <v>332</v>
       </c>
       <c r="D31" s="58" t="s">
-        <v>367</v>
+        <v>341</v>
       </c>
       <c r="E31" s="58" t="s">
-        <v>359</v>
-      </c>
-      <c r="F31" s="63" t="s">
-        <v>342</v>
-      </c>
+        <v>347</v>
+      </c>
+      <c r="F31" s="7"/>
       <c r="G31" s="8" t="s">
         <v>48</v>
       </c>
@@ -11723,7 +11809,7 @@
       <c r="IU31" s="43"/>
       <c r="IV31" s="43"/>
     </row>
-    <row r="32" spans="1:256" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="10">
         <v>42736</v>
       </c>
@@ -11732,18 +11818,18 @@
         <v>332</v>
       </c>
       <c r="D32" s="58" t="s">
-        <v>351</v>
+        <v>367</v>
       </c>
       <c r="E32" s="58" t="s">
-        <v>358</v>
-      </c>
-      <c r="F32" s="7"/>
-      <c r="G32" s="58" t="s">
-        <v>60</v>
-      </c>
-      <c r="H32" s="63" t="s">
-        <v>352</v>
-      </c>
+        <v>359</v>
+      </c>
+      <c r="F32" s="63" t="s">
+        <v>342</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H32" s="7"/>
       <c r="I32" s="7"/>
       <c r="J32" s="8" t="s">
         <v>27</v>
@@ -12004,16 +12090,18 @@
         <v>332</v>
       </c>
       <c r="D33" s="58" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="E33" s="58" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="F33" s="7"/>
-      <c r="G33" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="H33" s="7"/>
+      <c r="G33" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="H33" s="63" t="s">
+        <v>352</v>
+      </c>
       <c r="I33" s="7"/>
       <c r="J33" s="8" t="s">
         <v>27</v>
@@ -12265,23 +12353,23 @@
       <c r="IU33" s="43"/>
       <c r="IV33" s="43"/>
     </row>
-    <row r="34" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:256" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="10">
         <v>42736</v>
       </c>
       <c r="B34" s="10"/>
       <c r="C34" s="58" t="s">
-        <v>376</v>
+        <v>332</v>
       </c>
       <c r="D34" s="58" t="s">
-        <v>390</v>
+        <v>357</v>
       </c>
       <c r="E34" s="58" t="s">
-        <v>391</v>
-      </c>
-      <c r="F34" s="63"/>
+        <v>360</v>
+      </c>
+      <c r="F34" s="7"/>
       <c r="G34" s="8" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="H34" s="7"/>
       <c r="I34" s="7"/>
@@ -12544,10 +12632,10 @@
         <v>376</v>
       </c>
       <c r="D35" s="58" t="s">
-        <v>335</v>
+        <v>390</v>
       </c>
       <c r="E35" s="58" t="s">
-        <v>333</v>
+        <v>391</v>
       </c>
       <c r="F35" s="63"/>
       <c r="G35" s="8" t="s">
@@ -12814,10 +12902,10 @@
         <v>376</v>
       </c>
       <c r="D36" s="58" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E36" s="58" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F36" s="63"/>
       <c r="G36" s="8" t="s">
@@ -13084,10 +13172,10 @@
         <v>376</v>
       </c>
       <c r="D37" s="58" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E37" s="58" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="F37" s="63"/>
       <c r="G37" s="8" t="s">
@@ -13350,23 +13438,21 @@
         <v>42736</v>
       </c>
       <c r="B38" s="10"/>
-      <c r="C38" s="8" t="s">
-        <v>395</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="F38" s="7"/>
+      <c r="C38" s="58" t="s">
+        <v>376</v>
+      </c>
+      <c r="D38" s="58" t="s">
+        <v>339</v>
+      </c>
+      <c r="E38" s="58" t="s">
+        <v>343</v>
+      </c>
+      <c r="F38" s="63"/>
       <c r="G38" s="8" t="s">
         <v>48</v>
       </c>
       <c r="H38" s="7"/>
-      <c r="I38" s="7" t="s">
-        <v>398</v>
-      </c>
+      <c r="I38" s="7"/>
       <c r="J38" s="8" t="s">
         <v>27</v>
       </c>
@@ -13623,7 +13709,7 @@
       </c>
       <c r="B39" s="10"/>
       <c r="C39" s="8" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>66</v>
@@ -13636,7 +13722,9 @@
         <v>48</v>
       </c>
       <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
+      <c r="I39" s="7" t="s">
+        <v>398</v>
+      </c>
       <c r="J39" s="8" t="s">
         <v>27</v>
       </c>
@@ -13895,11 +13983,11 @@
       <c r="C40" s="8" t="s">
         <v>400</v>
       </c>
-      <c r="D40" s="58" t="s">
-        <v>336</v>
-      </c>
-      <c r="E40" s="58" t="s">
-        <v>334</v>
+      <c r="D40" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>67</v>
       </c>
       <c r="F40" s="7"/>
       <c r="G40" s="8" t="s">
@@ -14166,10 +14254,10 @@
         <v>400</v>
       </c>
       <c r="D41" s="58" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E41" s="58" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="F41" s="7"/>
       <c r="G41" s="8" t="s">
@@ -14427,6 +14515,276 @@
       <c r="IU41" s="43"/>
       <c r="IV41" s="43"/>
     </row>
+    <row r="42" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B42" s="10"/>
+      <c r="C42" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="D42" s="58" t="s">
+        <v>339</v>
+      </c>
+      <c r="E42" s="58" t="s">
+        <v>343</v>
+      </c>
+      <c r="F42" s="7"/>
+      <c r="G42" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K42" s="7"/>
+      <c r="L42" s="7"/>
+      <c r="M42" s="7"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="7"/>
+      <c r="P42" s="7"/>
+      <c r="Q42" s="7"/>
+      <c r="R42" s="43"/>
+      <c r="S42" s="43"/>
+      <c r="T42" s="43"/>
+      <c r="U42" s="43"/>
+      <c r="V42" s="43"/>
+      <c r="W42" s="43"/>
+      <c r="X42" s="43"/>
+      <c r="Y42" s="43"/>
+      <c r="Z42" s="43"/>
+      <c r="AA42" s="43"/>
+      <c r="AB42" s="43"/>
+      <c r="AC42" s="43"/>
+      <c r="AD42" s="43"/>
+      <c r="AE42" s="43"/>
+      <c r="AF42" s="43"/>
+      <c r="AG42" s="43"/>
+      <c r="AH42" s="43"/>
+      <c r="AI42" s="43"/>
+      <c r="AJ42" s="43"/>
+      <c r="AK42" s="43"/>
+      <c r="AL42" s="43"/>
+      <c r="AM42" s="43"/>
+      <c r="AN42" s="43"/>
+      <c r="AO42" s="43"/>
+      <c r="AP42" s="43"/>
+      <c r="AQ42" s="43"/>
+      <c r="AR42" s="43"/>
+      <c r="AS42" s="43"/>
+      <c r="AT42" s="43"/>
+      <c r="AU42" s="43"/>
+      <c r="AV42" s="43"/>
+      <c r="AW42" s="43"/>
+      <c r="AX42" s="43"/>
+      <c r="AY42" s="43"/>
+      <c r="AZ42" s="43"/>
+      <c r="BA42" s="43"/>
+      <c r="BB42" s="43"/>
+      <c r="BC42" s="43"/>
+      <c r="BD42" s="43"/>
+      <c r="BE42" s="43"/>
+      <c r="BF42" s="43"/>
+      <c r="BG42" s="43"/>
+      <c r="BH42" s="43"/>
+      <c r="BI42" s="43"/>
+      <c r="BJ42" s="43"/>
+      <c r="BK42" s="43"/>
+      <c r="BL42" s="43"/>
+      <c r="BM42" s="43"/>
+      <c r="BN42" s="43"/>
+      <c r="BO42" s="43"/>
+      <c r="BP42" s="43"/>
+      <c r="BQ42" s="43"/>
+      <c r="BR42" s="43"/>
+      <c r="BS42" s="43"/>
+      <c r="BT42" s="43"/>
+      <c r="BU42" s="43"/>
+      <c r="BV42" s="43"/>
+      <c r="BW42" s="43"/>
+      <c r="BX42" s="43"/>
+      <c r="BY42" s="43"/>
+      <c r="BZ42" s="43"/>
+      <c r="CA42" s="43"/>
+      <c r="CB42" s="43"/>
+      <c r="CC42" s="43"/>
+      <c r="CD42" s="43"/>
+      <c r="CE42" s="43"/>
+      <c r="CF42" s="43"/>
+      <c r="CG42" s="43"/>
+      <c r="CH42" s="43"/>
+      <c r="CI42" s="43"/>
+      <c r="CJ42" s="43"/>
+      <c r="CK42" s="43"/>
+      <c r="CL42" s="43"/>
+      <c r="CM42" s="43"/>
+      <c r="CN42" s="43"/>
+      <c r="CO42" s="43"/>
+      <c r="CP42" s="43"/>
+      <c r="CQ42" s="43"/>
+      <c r="CR42" s="43"/>
+      <c r="CS42" s="43"/>
+      <c r="CT42" s="43"/>
+      <c r="CU42" s="43"/>
+      <c r="CV42" s="43"/>
+      <c r="CW42" s="43"/>
+      <c r="CX42" s="43"/>
+      <c r="CY42" s="43"/>
+      <c r="CZ42" s="43"/>
+      <c r="DA42" s="43"/>
+      <c r="DB42" s="43"/>
+      <c r="DC42" s="43"/>
+      <c r="DD42" s="43"/>
+      <c r="DE42" s="43"/>
+      <c r="DF42" s="43"/>
+      <c r="DG42" s="43"/>
+      <c r="DH42" s="43"/>
+      <c r="DI42" s="43"/>
+      <c r="DJ42" s="43"/>
+      <c r="DK42" s="43"/>
+      <c r="DL42" s="43"/>
+      <c r="DM42" s="43"/>
+      <c r="DN42" s="43"/>
+      <c r="DO42" s="43"/>
+      <c r="DP42" s="43"/>
+      <c r="DQ42" s="43"/>
+      <c r="DR42" s="43"/>
+      <c r="DS42" s="43"/>
+      <c r="DT42" s="43"/>
+      <c r="DU42" s="43"/>
+      <c r="DV42" s="43"/>
+      <c r="DW42" s="43"/>
+      <c r="DX42" s="43"/>
+      <c r="DY42" s="43"/>
+      <c r="DZ42" s="43"/>
+      <c r="EA42" s="43"/>
+      <c r="EB42" s="43"/>
+      <c r="EC42" s="43"/>
+      <c r="ED42" s="43"/>
+      <c r="EE42" s="43"/>
+      <c r="EF42" s="43"/>
+      <c r="EG42" s="43"/>
+      <c r="EH42" s="43"/>
+      <c r="EI42" s="43"/>
+      <c r="EJ42" s="43"/>
+      <c r="EK42" s="43"/>
+      <c r="EL42" s="43"/>
+      <c r="EM42" s="43"/>
+      <c r="EN42" s="43"/>
+      <c r="EO42" s="43"/>
+      <c r="EP42" s="43"/>
+      <c r="EQ42" s="43"/>
+      <c r="ER42" s="43"/>
+      <c r="ES42" s="43"/>
+      <c r="ET42" s="43"/>
+      <c r="EU42" s="43"/>
+      <c r="EV42" s="43"/>
+      <c r="EW42" s="43"/>
+      <c r="EX42" s="43"/>
+      <c r="EY42" s="43"/>
+      <c r="EZ42" s="43"/>
+      <c r="FA42" s="43"/>
+      <c r="FB42" s="43"/>
+      <c r="FC42" s="43"/>
+      <c r="FD42" s="43"/>
+      <c r="FE42" s="43"/>
+      <c r="FF42" s="43"/>
+      <c r="FG42" s="43"/>
+      <c r="FH42" s="43"/>
+      <c r="FI42" s="43"/>
+      <c r="FJ42" s="43"/>
+      <c r="FK42" s="43"/>
+      <c r="FL42" s="43"/>
+      <c r="FM42" s="43"/>
+      <c r="FN42" s="43"/>
+      <c r="FO42" s="43"/>
+      <c r="FP42" s="43"/>
+      <c r="FQ42" s="43"/>
+      <c r="FR42" s="43"/>
+      <c r="FS42" s="43"/>
+      <c r="FT42" s="43"/>
+      <c r="FU42" s="43"/>
+      <c r="FV42" s="43"/>
+      <c r="FW42" s="43"/>
+      <c r="FX42" s="43"/>
+      <c r="FY42" s="43"/>
+      <c r="FZ42" s="43"/>
+      <c r="GA42" s="43"/>
+      <c r="GB42" s="43"/>
+      <c r="GC42" s="43"/>
+      <c r="GD42" s="43"/>
+      <c r="GE42" s="43"/>
+      <c r="GF42" s="43"/>
+      <c r="GG42" s="43"/>
+      <c r="GH42" s="43"/>
+      <c r="GI42" s="43"/>
+      <c r="GJ42" s="43"/>
+      <c r="GK42" s="43"/>
+      <c r="GL42" s="43"/>
+      <c r="GM42" s="43"/>
+      <c r="GN42" s="43"/>
+      <c r="GO42" s="43"/>
+      <c r="GP42" s="43"/>
+      <c r="GQ42" s="43"/>
+      <c r="GR42" s="43"/>
+      <c r="GS42" s="43"/>
+      <c r="GT42" s="43"/>
+      <c r="GU42" s="43"/>
+      <c r="GV42" s="43"/>
+      <c r="GW42" s="43"/>
+      <c r="GX42" s="43"/>
+      <c r="GY42" s="43"/>
+      <c r="GZ42" s="43"/>
+      <c r="HA42" s="43"/>
+      <c r="HB42" s="43"/>
+      <c r="HC42" s="43"/>
+      <c r="HD42" s="43"/>
+      <c r="HE42" s="43"/>
+      <c r="HF42" s="43"/>
+      <c r="HG42" s="43"/>
+      <c r="HH42" s="43"/>
+      <c r="HI42" s="43"/>
+      <c r="HJ42" s="43"/>
+      <c r="HK42" s="43"/>
+      <c r="HL42" s="43"/>
+      <c r="HM42" s="43"/>
+      <c r="HN42" s="43"/>
+      <c r="HO42" s="43"/>
+      <c r="HP42" s="43"/>
+      <c r="HQ42" s="43"/>
+      <c r="HR42" s="43"/>
+      <c r="HS42" s="43"/>
+      <c r="HT42" s="43"/>
+      <c r="HU42" s="43"/>
+      <c r="HV42" s="43"/>
+      <c r="HW42" s="43"/>
+      <c r="HX42" s="43"/>
+      <c r="HY42" s="43"/>
+      <c r="HZ42" s="43"/>
+      <c r="IA42" s="43"/>
+      <c r="IB42" s="43"/>
+      <c r="IC42" s="43"/>
+      <c r="ID42" s="43"/>
+      <c r="IE42" s="43"/>
+      <c r="IF42" s="43"/>
+      <c r="IG42" s="43"/>
+      <c r="IH42" s="43"/>
+      <c r="II42" s="43"/>
+      <c r="IJ42" s="43"/>
+      <c r="IK42" s="43"/>
+      <c r="IL42" s="43"/>
+      <c r="IM42" s="43"/>
+      <c r="IN42" s="43"/>
+      <c r="IO42" s="43"/>
+      <c r="IP42" s="43"/>
+      <c r="IQ42" s="43"/>
+      <c r="IR42" s="43"/>
+      <c r="IS42" s="43"/>
+      <c r="IT42" s="43"/>
+      <c r="IU42" s="43"/>
+      <c r="IV42" s="43"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -14438,10 +14796,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:R27"/>
+  <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="B8" sqref="A8:XFD8"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -14909,23 +15267,23 @@
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="8" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="8" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="H14" s="8"/>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
       <c r="K14" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
@@ -14944,20 +15302,20 @@
         <v>114</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="8" t="s">
-        <v>116</v>
+        <v>12</v>
       </c>
       <c r="H15" s="8"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
       <c r="K15" s="8" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>
@@ -14976,20 +15334,20 @@
         <v>114</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>51</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H16" s="8"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
       <c r="K16" s="8" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="L16" s="7"/>
       <c r="M16" s="7"/>
@@ -15005,23 +15363,23 @@
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="8" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="8" t="s">
-        <v>12</v>
+        <v>118</v>
       </c>
       <c r="H17" s="8"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L17" s="7"/>
       <c r="M17" s="7"/>
@@ -15040,20 +15398,20 @@
         <v>119</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="8" t="s">
-        <v>116</v>
+        <v>12</v>
       </c>
       <c r="H18" s="8"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
       <c r="K18" s="8" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="L18" s="7"/>
       <c r="M18" s="7"/>
@@ -15063,7 +15421,7 @@
       <c r="Q18" s="7"/>
       <c r="R18" s="7"/>
     </row>
-    <row r="19" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="10">
         <v>42736</v>
       </c>
@@ -15072,20 +15430,20 @@
         <v>119</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>51</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H19" s="8"/>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
       <c r="K19" s="8" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="L19" s="7"/>
       <c r="M19" s="7"/>
@@ -15095,29 +15453,29 @@
       <c r="Q19" s="7"/>
       <c r="R19" s="7"/>
     </row>
-    <row r="20" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="10">
         <v>42736</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="8" t="s">
-        <v>299</v>
+        <v>119</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>301</v>
+        <v>117</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="8" t="s">
-        <v>300</v>
+        <v>118</v>
       </c>
       <c r="H20" s="8"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
       <c r="K20" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L20" s="7"/>
       <c r="M20" s="7"/>
@@ -15136,16 +15494,14 @@
         <v>299</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>306</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="F21" s="7"/>
       <c r="G21" s="8" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="H21" s="8"/>
       <c r="I21" s="7"/>
@@ -15170,14 +15526,16 @@
         <v>299</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F22" s="7"/>
+        <v>60</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>306</v>
+      </c>
       <c r="G22" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H22" s="8"/>
       <c r="I22" s="7"/>
@@ -15193,23 +15551,23 @@
       <c r="Q22" s="7"/>
       <c r="R22" s="7"/>
     </row>
-    <row r="23" spans="1:18" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="10">
         <v>42736</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="8" t="s">
-        <v>288</v>
+        <v>299</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>289</v>
+        <v>302</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="8" t="s">
-        <v>290</v>
+        <v>305</v>
       </c>
       <c r="H23" s="8"/>
       <c r="I23" s="7"/>
@@ -15225,7 +15583,7 @@
       <c r="Q23" s="7"/>
       <c r="R23" s="7"/>
     </row>
-    <row r="24" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:18" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="10">
         <v>42736</v>
       </c>
@@ -15234,14 +15592,14 @@
         <v>288</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>48</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="8" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="H24" s="8"/>
       <c r="I24" s="7"/>
@@ -15257,7 +15615,7 @@
       <c r="Q24" s="7"/>
       <c r="R24" s="7"/>
     </row>
-    <row r="25" spans="1:18" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="10">
         <v>42736</v>
       </c>
@@ -15266,14 +15624,14 @@
         <v>288</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>48</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="8" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="H25" s="8"/>
       <c r="I25" s="7"/>
@@ -15289,7 +15647,7 @@
       <c r="Q25" s="7"/>
       <c r="R25" s="7"/>
     </row>
-    <row r="26" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:18" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="10">
         <v>42736</v>
       </c>
@@ -15298,14 +15656,14 @@
         <v>288</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>48</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="8" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="H26" s="8"/>
       <c r="I26" s="7"/>
@@ -15330,16 +15688,14 @@
         <v>288</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="G27" s="58" t="s">
-        <v>321</v>
+        <v>48</v>
+      </c>
+      <c r="F27" s="7"/>
+      <c r="G27" s="8" t="s">
+        <v>296</v>
       </c>
       <c r="H27" s="8"/>
       <c r="I27" s="7"/>
@@ -15354,6 +15710,40 @@
       <c r="P27" s="7"/>
       <c r="Q27" s="7"/>
       <c r="R27" s="7"/>
+    </row>
+    <row r="28" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B28" s="10"/>
+      <c r="C28" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="G28" s="58" t="s">
+        <v>321</v>
+      </c>
+      <c r="H28" s="8"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
@@ -15697,10 +16087,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView showGridLines="0" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -15715,7 +16105,8 @@
     <col min="9" max="9" width="21" style="18" customWidth="1"/>
     <col min="10" max="10" width="30.33203125" style="18" customWidth="1"/>
     <col min="11" max="11" width="16.33203125" style="18" customWidth="1"/>
-    <col min="12" max="14" width="8.83203125" style="18" customWidth="1"/>
+    <col min="12" max="12" width="8.83203125" style="79" customWidth="1"/>
+    <col min="13" max="14" width="8.83203125" style="18" customWidth="1"/>
     <col min="15" max="256" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -15739,7 +16130,7 @@
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
+      <c r="L1" s="74"/>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
     </row>
@@ -15777,7 +16168,9 @@
       <c r="K2" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="L2" s="7"/>
+      <c r="L2" s="75" t="s">
+        <v>416</v>
+      </c>
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
     </row>
@@ -15815,7 +16208,9 @@
       <c r="K3" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="L3" s="6"/>
+      <c r="L3" s="76" t="s">
+        <v>417</v>
+      </c>
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
     </row>
@@ -15847,39 +16242,41 @@
       </c>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
+      <c r="L4" s="77"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
     </row>
-    <row r="5" spans="1:14" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="10">
         <v>42736</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="8" t="s">
-        <v>275</v>
+        <v>399</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="E5" s="58" t="s">
-        <v>156</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>156</v>
+      <c r="E5" s="81" t="s">
+        <v>419</v>
+      </c>
+      <c r="F5" s="58" t="s">
+        <v>415</v>
       </c>
       <c r="G5" s="6">
         <v>1</v>
       </c>
-      <c r="H5" s="58" t="s">
-        <v>369</v>
+      <c r="H5" s="81" t="s">
+        <v>420</v>
       </c>
       <c r="I5" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
+      <c r="L5" s="78" t="s">
+        <v>418</v>
+      </c>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
     </row>
@@ -15903,47 +16300,47 @@
       <c r="G6" s="6">
         <v>1</v>
       </c>
-      <c r="H6" s="8" t="s">
-        <v>276</v>
+      <c r="H6" s="58" t="s">
+        <v>369</v>
       </c>
       <c r="I6" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
+      <c r="L6" s="74"/>
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
     </row>
-    <row r="7" spans="1:14" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:14" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="10">
         <v>42736</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="58" t="s">
-        <v>332</v>
+      <c r="C7" s="8" t="s">
+        <v>275</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>157</v>
       </c>
       <c r="E7" s="58" t="s">
-        <v>325</v>
-      </c>
-      <c r="F7" s="58" t="s">
-        <v>325</v>
+        <v>156</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>156</v>
       </c>
       <c r="G7" s="6">
-        <v>2</v>
-      </c>
-      <c r="H7" s="58" t="s">
-        <v>337</v>
+        <v>1</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>276</v>
       </c>
       <c r="I7" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
+      <c r="L7" s="74"/>
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
     </row>
@@ -15968,14 +16365,14 @@
         <v>2</v>
       </c>
       <c r="H8" s="58" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="I8" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
+      <c r="L8" s="74"/>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
     </row>
@@ -16000,14 +16397,14 @@
         <v>2</v>
       </c>
       <c r="H9" s="58" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="I9" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
+      <c r="L9" s="78"/>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
     </row>
@@ -16023,23 +16420,23 @@
         <v>157</v>
       </c>
       <c r="E10" s="58" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="F10" s="58" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="G10" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H10" s="58" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="I10" s="6">
         <v>1</v>
       </c>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
+      <c r="L10" s="74"/>
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
     </row>
@@ -16055,23 +16452,22 @@
         <v>157</v>
       </c>
       <c r="E11" s="58" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F11" s="58" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G11" s="6">
-        <v>3</v>
-      </c>
-      <c r="H11" s="60" t="s">
-        <v>367</v>
+        <v>1</v>
+      </c>
+      <c r="H11" s="58" t="s">
+        <v>335</v>
       </c>
       <c r="I11" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J11" s="7"/>
-      <c r="K11" s="66"/>
-      <c r="L11" s="7"/>
+      <c r="K11" s="7"/>
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
     </row>
@@ -16095,15 +16491,15 @@
       <c r="G12" s="6">
         <v>3</v>
       </c>
-      <c r="H12" s="64" t="s">
-        <v>351</v>
+      <c r="H12" s="60" t="s">
+        <v>367</v>
       </c>
       <c r="I12" s="6">
         <v>3</v>
       </c>
       <c r="J12" s="7"/>
       <c r="K12" s="66"/>
-      <c r="L12" s="7"/>
+      <c r="L12" s="74"/>
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
     </row>
@@ -16128,14 +16524,14 @@
         <v>3</v>
       </c>
       <c r="H13" s="64" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="I13" s="6">
         <v>3</v>
       </c>
       <c r="J13" s="7"/>
       <c r="K13" s="66"/>
-      <c r="L13" s="7"/>
+      <c r="L13" s="74"/>
       <c r="M13" s="7"/>
       <c r="N13" s="7"/>
     </row>
@@ -16151,25 +16547,23 @@
         <v>157</v>
       </c>
       <c r="E14" s="58" t="s">
-        <v>364</v>
+        <v>326</v>
       </c>
       <c r="F14" s="58" t="s">
-        <v>361</v>
+        <v>326</v>
       </c>
       <c r="G14" s="6">
-        <v>4</v>
-      </c>
-      <c r="H14" s="58" t="s">
-        <v>338</v>
+        <v>3</v>
+      </c>
+      <c r="H14" s="64" t="s">
+        <v>357</v>
       </c>
       <c r="I14" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J14" s="7"/>
-      <c r="K14" s="60" t="s">
-        <v>373</v>
-      </c>
-      <c r="L14" s="7"/>
+      <c r="K14" s="66"/>
+      <c r="L14" s="74"/>
       <c r="M14" s="7"/>
       <c r="N14" s="7"/>
     </row>
@@ -16185,25 +16579,25 @@
         <v>157</v>
       </c>
       <c r="E15" s="58" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F15" s="58" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G15" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H15" s="58" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="I15" s="6">
         <v>1</v>
       </c>
       <c r="J15" s="7"/>
-      <c r="K15" s="64" t="s">
-        <v>375</v>
-      </c>
-      <c r="L15" s="7"/>
+      <c r="K15" s="60" t="s">
+        <v>373</v>
+      </c>
+      <c r="L15" s="74"/>
       <c r="M15" s="7"/>
       <c r="N15" s="7"/>
     </row>
@@ -16219,57 +16613,59 @@
         <v>157</v>
       </c>
       <c r="E16" s="58" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F16" s="58" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G16" s="6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H16" s="58" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I16" s="6">
         <v>1</v>
       </c>
       <c r="J16" s="7"/>
       <c r="K16" s="64" t="s">
-        <v>374</v>
-      </c>
-      <c r="L16" s="7"/>
+        <v>375</v>
+      </c>
+      <c r="L16" s="74"/>
       <c r="M16" s="7"/>
       <c r="N16" s="7"/>
     </row>
-    <row r="17" spans="1:14" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="10">
         <v>42736</v>
       </c>
       <c r="B17" s="10"/>
-      <c r="C17" s="8" t="s">
-        <v>285</v>
+      <c r="C17" s="58" t="s">
+        <v>332</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="E17" s="8" t="s">
-        <v>315</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>314</v>
+      <c r="E17" s="58" t="s">
+        <v>366</v>
+      </c>
+      <c r="F17" s="58" t="s">
+        <v>363</v>
       </c>
       <c r="G17" s="6">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H17" s="58" t="s">
-        <v>313</v>
+        <v>341</v>
       </c>
       <c r="I17" s="6">
         <v>1</v>
       </c>
       <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
+      <c r="K17" s="64" t="s">
+        <v>374</v>
+      </c>
+      <c r="L17" s="74"/>
       <c r="M17" s="7"/>
       <c r="N17" s="7"/>
     </row>
@@ -16279,29 +16675,29 @@
       </c>
       <c r="B18" s="10"/>
       <c r="C18" s="8" t="s">
-        <v>376</v>
+        <v>285</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="E18" s="19" t="s">
-        <v>392</v>
+      <c r="E18" s="8" t="s">
+        <v>315</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>392</v>
+        <v>314</v>
       </c>
       <c r="G18" s="6">
         <v>1</v>
       </c>
-      <c r="H18" s="8" t="s">
-        <v>390</v>
+      <c r="H18" s="58" t="s">
+        <v>313</v>
       </c>
       <c r="I18" s="6">
         <v>1</v>
       </c>
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
+      <c r="L18" s="74"/>
       <c r="M18" s="7"/>
       <c r="N18" s="7"/>
     </row>
@@ -16326,14 +16722,14 @@
         <v>1</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>335</v>
+        <v>390</v>
       </c>
       <c r="I19" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
+      <c r="L19" s="74"/>
       <c r="M19" s="7"/>
       <c r="N19" s="7"/>
     </row>
@@ -16358,14 +16754,14 @@
         <v>1</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I20" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
+      <c r="L20" s="74"/>
       <c r="M20" s="7"/>
       <c r="N20" s="7"/>
     </row>
@@ -16390,14 +16786,14 @@
         <v>1</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="I21" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
+      <c r="L21" s="74"/>
       <c r="M21" s="7"/>
       <c r="N21" s="7"/>
     </row>
@@ -16407,48 +16803,48 @@
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="8" t="s">
-        <v>395</v>
+        <v>376</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>157</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>156</v>
+        <v>392</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>156</v>
+        <v>392</v>
       </c>
       <c r="G22" s="6">
         <v>1</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>66</v>
+        <v>339</v>
       </c>
       <c r="I22" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
+      <c r="L22" s="74"/>
       <c r="M22" s="7"/>
       <c r="N22" s="7"/>
     </row>
-    <row r="23" spans="1:14" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:14" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10">
         <v>42736</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="8" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="E23" s="58" t="s">
-        <v>364</v>
-      </c>
-      <c r="F23" s="58" t="s">
-        <v>361</v>
+      <c r="E23" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>156</v>
       </c>
       <c r="G23" s="6">
         <v>1</v>
@@ -16460,10 +16856,8 @@
         <v>1</v>
       </c>
       <c r="J23" s="7"/>
-      <c r="K23" s="60" t="s">
-        <v>403</v>
-      </c>
-      <c r="L23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="74"/>
       <c r="M23" s="7"/>
       <c r="N23" s="7"/>
     </row>
@@ -16488,20 +16882,62 @@
         <v>1</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>339</v>
+        <v>66</v>
       </c>
       <c r="I24" s="6">
         <v>1</v>
       </c>
-      <c r="J24" s="60" t="s">
-        <v>407</v>
-      </c>
-      <c r="K24" s="60"/>
-      <c r="L24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="60" t="s">
+        <v>403</v>
+      </c>
+      <c r="L24" s="74"/>
       <c r="M24" s="7"/>
       <c r="N24" s="7"/>
     </row>
-    <row r="27" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="25" spans="1:14" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B25" s="10"/>
+      <c r="C25" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E25" s="58" t="s">
+        <v>364</v>
+      </c>
+      <c r="F25" s="58" t="s">
+        <v>361</v>
+      </c>
+      <c r="G25" s="6">
+        <v>1</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="I25" s="6">
+        <v>1</v>
+      </c>
+      <c r="J25" s="60" t="s">
+        <v>407</v>
+      </c>
+      <c r="K25" s="60"/>
+      <c r="L25" s="74"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+    </row>
+    <row r="26" spans="1:14" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L26" s="74"/>
+    </row>
+    <row r="27" spans="1:14" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L27" s="74"/>
+    </row>
+    <row r="28" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L28" s="74"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -16516,7 +16952,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -16868,8 +17304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -17565,8 +18001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AB42"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -17732,7 +18168,9 @@
       <c r="O3" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="P3" s="7"/>
+      <c r="P3" s="76" t="s">
+        <v>417</v>
+      </c>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
@@ -17811,7 +18249,7 @@
         <v>68</v>
       </c>
       <c r="F5" s="23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>218</v>
@@ -17857,8 +18295,8 @@
       <c r="D6" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>71</v>
+      <c r="E6" s="81" t="s">
+        <v>420</v>
       </c>
       <c r="F6" s="23">
         <v>1</v>
@@ -17882,8 +18320,9 @@
         <v>195</v>
       </c>
       <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
+      <c r="P6" s="78" t="s">
+        <v>418</v>
+      </c>
       <c r="R6" s="7"/>
       <c r="S6" s="7"/>
       <c r="T6" s="7"/>
@@ -17917,7 +18356,7 @@
         <v>218</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>219</v>
+        <v>422</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>220</v>
@@ -17967,7 +18406,7 @@
         <v>218</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>219</v>
+        <v>422</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>220</v>
@@ -18017,7 +18456,7 @@
         <v>218</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>219</v>
+        <v>422</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>220</v>
@@ -18067,7 +18506,7 @@
         <v>218</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>219</v>
+        <v>422</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>220</v>
@@ -18117,7 +18556,7 @@
         <v>218</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>219</v>
+        <v>422</v>
       </c>
       <c r="I11" s="8" t="s">
         <v>220</v>
@@ -18167,7 +18606,7 @@
         <v>218</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>219</v>
+        <v>422</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>220</v>
@@ -18217,7 +18656,7 @@
         <v>218</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>219</v>
+        <v>422</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>220</v>
@@ -18267,7 +18706,7 @@
         <v>218</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>219</v>
+        <v>422</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>220</v>
@@ -18317,7 +18756,7 @@
         <v>218</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>219</v>
+        <v>422</v>
       </c>
       <c r="I15" s="8" t="s">
         <v>220</v>
@@ -18367,7 +18806,7 @@
         <v>218</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>219</v>
+        <v>422</v>
       </c>
       <c r="I16" s="8" t="s">
         <v>220</v>

</xml_diff>

<commit_message>
Changed Tab name to match excel file
</commit_message>
<xml_diff>
--- a/test/resources/definitionsFiles/fe-automation-definition-v03.xlsx
+++ b/test/resources/definitionsFiles/fe-automation-definition-v03.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohammedanaskhatri/project/ccd-case-management-web/test/resources/definitionsFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE082E49-E1DF-014A-80C3-5F119EDA11AA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C001ED8-B619-2B47-BD70-DC780F997D22}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -1361,9 +1361,6 @@
     <t>Case Reference</t>
   </si>
   <si>
-    <t>Reference Collecrions</t>
-  </si>
-  <si>
     <t>MaxLength: 1000</t>
   </si>
   <si>
@@ -1392,6 +1389,9 @@
   </si>
   <si>
     <t>DynamicList1212</t>
+  </si>
+  <si>
+    <t>Reference Collections</t>
   </si>
 </sst>
 </file>
@@ -4884,7 +4884,7 @@
         <v>397</v>
       </c>
       <c r="D4" s="83" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E4" t="s">
         <v>269</v>
@@ -6977,8 +6977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:IV43"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7767,10 +7767,10 @@
         <v>397</v>
       </c>
       <c r="D17" s="81" t="s">
+        <v>417</v>
+      </c>
+      <c r="E17" s="81" t="s">
         <v>418</v>
-      </c>
-      <c r="E17" s="81" t="s">
-        <v>419</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="80" t="s">
@@ -8039,14 +8039,14 @@
         <v>397</v>
       </c>
       <c r="D18" s="81" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E18" s="81" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="80" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H18" s="81"/>
       <c r="I18" s="7"/>
@@ -15071,7 +15071,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="K4" sqref="K4:K7"/>
     </sheetView>
   </sheetViews>
@@ -16330,7 +16330,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -16410,7 +16410,7 @@
         <v>145</v>
       </c>
       <c r="L2" s="75" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
@@ -16450,7 +16450,7 @@
         <v>152</v>
       </c>
       <c r="L3" s="76" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
@@ -16499,16 +16499,16 @@
         <v>155</v>
       </c>
       <c r="E5" s="81" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F5" s="58" t="s">
-        <v>413</v>
+        <v>423</v>
       </c>
       <c r="G5" s="6">
         <v>1</v>
       </c>
       <c r="H5" s="81" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="I5" s="6">
         <v>1</v>
@@ -16516,7 +16516,7 @@
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
       <c r="L5" s="78" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
@@ -18410,7 +18410,7 @@
         <v>215</v>
       </c>
       <c r="P3" s="76" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
@@ -18537,7 +18537,7 @@
         <v>191</v>
       </c>
       <c r="E6" s="81" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F6" s="23">
         <v>1</v>
@@ -18562,7 +18562,7 @@
       </c>
       <c r="O6" s="7"/>
       <c r="P6" s="78" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="R6" s="7"/>
       <c r="S6" s="7"/>
@@ -18597,7 +18597,7 @@
         <v>216</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>218</v>
@@ -18647,7 +18647,7 @@
         <v>216</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>218</v>
@@ -18697,7 +18697,7 @@
         <v>216</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>218</v>
@@ -18747,7 +18747,7 @@
         <v>216</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>218</v>
@@ -18797,7 +18797,7 @@
         <v>216</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="I11" s="8" t="s">
         <v>218</v>
@@ -18847,7 +18847,7 @@
         <v>216</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>218</v>
@@ -18897,7 +18897,7 @@
         <v>216</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>218</v>
@@ -18947,7 +18947,7 @@
         <v>216</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>218</v>
@@ -18997,7 +18997,7 @@
         <v>216</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="I15" s="8" t="s">
         <v>218</v>
@@ -19047,7 +19047,7 @@
         <v>216</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="I16" s="8" t="s">
         <v>218</v>

</xml_diff>

<commit_message>
RDM-4184 Update func tests and spreadsheet to reflect removing of the fixed History tab.
</commit_message>
<xml_diff>
--- a/test/resources/definitionsFiles/fe-automation-definition-v03.xlsx
+++ b/test/resources/definitionsFiles/fe-automation-definition-v03.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dev/Documents/Definition Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrzejfolga/src/ccd/temp/ccd-case-management-web/test/resources/definitionsFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C03B15-2E2B-B642-8670-12D7B70880B4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" firstSheet="7" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -33,7 +32,7 @@
     <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId18"/>
     <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -46,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1704" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1718" uniqueCount="419">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1365,17 +1364,29 @@
   </si>
   <si>
     <t>Case Reference</t>
+  </si>
+  <si>
+    <t>history</t>
+  </si>
+  <si>
+    <t>Case History</t>
+  </si>
+  <si>
+    <t>CaseHistoryViewer</t>
+  </si>
+  <si>
+    <t>CaseHistory</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;DD/&quot;mm&quot;/YYYY&quot;"/>
     <numFmt numFmtId="165" formatCode="&quot;D/&quot;m&quot;/YY&quot;"/>
   </numFmts>
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -1556,6 +1567,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1663,12 +1681,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1753,11 +1773,15 @@
     <xf numFmtId="164" fontId="29" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="29" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="23" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="23" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7"/>
@@ -2914,7 +2938,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3098,7 +3122,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3596,7 +3620,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3857,7 +3881,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -4067,7 +4091,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -4355,7 +4379,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -4500,7 +4524,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-0D00-000003000000}"/>
+    <hyperlink ref="C4" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -4511,7 +4535,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -4707,11 +4731,11 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:K41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:XFD38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5571,11 +5595,11 @@
         <v>42736</v>
       </c>
       <c r="B38" s="10"/>
-      <c r="C38" s="8" t="s">
-        <v>395</v>
+      <c r="C38" s="58" t="s">
+        <v>376</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>66</v>
+        <v>418</v>
       </c>
       <c r="E38" t="s">
         <v>271</v>
@@ -5595,7 +5619,7 @@
       </c>
       <c r="B39" s="10"/>
       <c r="C39" s="8" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>66</v>
@@ -5620,8 +5644,8 @@
       <c r="C40" s="8" t="s">
         <v>400</v>
       </c>
-      <c r="D40" s="58" t="s">
-        <v>336</v>
+      <c r="D40" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="E40" t="s">
         <v>271</v>
@@ -5644,7 +5668,7 @@
         <v>400</v>
       </c>
       <c r="D41" s="58" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E41" t="s">
         <v>271</v>
@@ -5657,6 +5681,29 @@
       <c r="I41" s="7"/>
       <c r="J41" s="7"/>
       <c r="K41" s="7"/>
+    </row>
+    <row r="42" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B42" s="10"/>
+      <c r="C42" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="D42" s="58" t="s">
+        <v>339</v>
+      </c>
+      <c r="E42" t="s">
+        <v>271</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="G42" s="8"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
@@ -5668,7 +5715,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5784,7 +5831,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
@@ -6182,7 +6229,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -6560,7 +6607,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
@@ -6874,7 +6921,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G4" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="G4" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -6885,11 +6932,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:IV41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV43"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+    <sheetView showGridLines="0" topLeftCell="C3" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -13349,34 +13396,32 @@
       <c r="A38" s="10">
         <v>42736</v>
       </c>
-      <c r="B38" s="10"/>
-      <c r="C38" s="8" t="s">
-        <v>395</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="F38" s="7"/>
-      <c r="G38" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7" t="s">
-        <v>398</v>
-      </c>
-      <c r="J38" s="8" t="s">
+      <c r="B38" s="74"/>
+      <c r="C38" s="58" t="s">
+        <v>376</v>
+      </c>
+      <c r="D38" s="73" t="s">
+        <v>418</v>
+      </c>
+      <c r="E38" s="73" t="s">
+        <v>416</v>
+      </c>
+      <c r="F38" s="75"/>
+      <c r="G38" s="73" t="s">
+        <v>417</v>
+      </c>
+      <c r="H38" s="75"/>
+      <c r="I38" s="75"/>
+      <c r="J38" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="K38" s="7"/>
-      <c r="L38" s="7"/>
-      <c r="M38" s="7"/>
-      <c r="N38" s="7"/>
-      <c r="O38" s="7"/>
-      <c r="P38" s="7"/>
-      <c r="Q38" s="7"/>
+      <c r="K38" s="75"/>
+      <c r="L38" s="75"/>
+      <c r="M38" s="75"/>
+      <c r="N38" s="75"/>
+      <c r="O38" s="75"/>
+      <c r="P38" s="75"/>
+      <c r="Q38" s="75"/>
       <c r="R38" s="43"/>
       <c r="S38" s="43"/>
       <c r="T38" s="43"/>
@@ -13623,7 +13668,7 @@
       </c>
       <c r="B39" s="10"/>
       <c r="C39" s="8" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>66</v>
@@ -13636,7 +13681,9 @@
         <v>48</v>
       </c>
       <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
+      <c r="I39" s="7" t="s">
+        <v>398</v>
+      </c>
       <c r="J39" s="8" t="s">
         <v>27</v>
       </c>
@@ -13895,11 +13942,11 @@
       <c r="C40" s="8" t="s">
         <v>400</v>
       </c>
-      <c r="D40" s="58" t="s">
-        <v>336</v>
-      </c>
-      <c r="E40" s="58" t="s">
-        <v>334</v>
+      <c r="D40" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>67</v>
       </c>
       <c r="F40" s="7"/>
       <c r="G40" s="8" t="s">
@@ -14166,10 +14213,10 @@
         <v>400</v>
       </c>
       <c r="D41" s="58" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E41" s="58" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="F41" s="7"/>
       <c r="G41" s="8" t="s">
@@ -14427,6 +14474,534 @@
       <c r="IU41" s="43"/>
       <c r="IV41" s="43"/>
     </row>
+    <row r="42" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B42" s="10"/>
+      <c r="C42" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="D42" s="58" t="s">
+        <v>339</v>
+      </c>
+      <c r="E42" s="58" t="s">
+        <v>343</v>
+      </c>
+      <c r="F42" s="7"/>
+      <c r="G42" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K42" s="7"/>
+      <c r="L42" s="7"/>
+      <c r="M42" s="7"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="7"/>
+      <c r="P42" s="7"/>
+      <c r="Q42" s="7"/>
+      <c r="R42" s="43"/>
+      <c r="S42" s="43"/>
+      <c r="T42" s="43"/>
+      <c r="U42" s="43"/>
+      <c r="V42" s="43"/>
+      <c r="W42" s="43"/>
+      <c r="X42" s="43"/>
+      <c r="Y42" s="43"/>
+      <c r="Z42" s="43"/>
+      <c r="AA42" s="43"/>
+      <c r="AB42" s="43"/>
+      <c r="AC42" s="43"/>
+      <c r="AD42" s="43"/>
+      <c r="AE42" s="43"/>
+      <c r="AF42" s="43"/>
+      <c r="AG42" s="43"/>
+      <c r="AH42" s="43"/>
+      <c r="AI42" s="43"/>
+      <c r="AJ42" s="43"/>
+      <c r="AK42" s="43"/>
+      <c r="AL42" s="43"/>
+      <c r="AM42" s="43"/>
+      <c r="AN42" s="43"/>
+      <c r="AO42" s="43"/>
+      <c r="AP42" s="43"/>
+      <c r="AQ42" s="43"/>
+      <c r="AR42" s="43"/>
+      <c r="AS42" s="43"/>
+      <c r="AT42" s="43"/>
+      <c r="AU42" s="43"/>
+      <c r="AV42" s="43"/>
+      <c r="AW42" s="43"/>
+      <c r="AX42" s="43"/>
+      <c r="AY42" s="43"/>
+      <c r="AZ42" s="43"/>
+      <c r="BA42" s="43"/>
+      <c r="BB42" s="43"/>
+      <c r="BC42" s="43"/>
+      <c r="BD42" s="43"/>
+      <c r="BE42" s="43"/>
+      <c r="BF42" s="43"/>
+      <c r="BG42" s="43"/>
+      <c r="BH42" s="43"/>
+      <c r="BI42" s="43"/>
+      <c r="BJ42" s="43"/>
+      <c r="BK42" s="43"/>
+      <c r="BL42" s="43"/>
+      <c r="BM42" s="43"/>
+      <c r="BN42" s="43"/>
+      <c r="BO42" s="43"/>
+      <c r="BP42" s="43"/>
+      <c r="BQ42" s="43"/>
+      <c r="BR42" s="43"/>
+      <c r="BS42" s="43"/>
+      <c r="BT42" s="43"/>
+      <c r="BU42" s="43"/>
+      <c r="BV42" s="43"/>
+      <c r="BW42" s="43"/>
+      <c r="BX42" s="43"/>
+      <c r="BY42" s="43"/>
+      <c r="BZ42" s="43"/>
+      <c r="CA42" s="43"/>
+      <c r="CB42" s="43"/>
+      <c r="CC42" s="43"/>
+      <c r="CD42" s="43"/>
+      <c r="CE42" s="43"/>
+      <c r="CF42" s="43"/>
+      <c r="CG42" s="43"/>
+      <c r="CH42" s="43"/>
+      <c r="CI42" s="43"/>
+      <c r="CJ42" s="43"/>
+      <c r="CK42" s="43"/>
+      <c r="CL42" s="43"/>
+      <c r="CM42" s="43"/>
+      <c r="CN42" s="43"/>
+      <c r="CO42" s="43"/>
+      <c r="CP42" s="43"/>
+      <c r="CQ42" s="43"/>
+      <c r="CR42" s="43"/>
+      <c r="CS42" s="43"/>
+      <c r="CT42" s="43"/>
+      <c r="CU42" s="43"/>
+      <c r="CV42" s="43"/>
+      <c r="CW42" s="43"/>
+      <c r="CX42" s="43"/>
+      <c r="CY42" s="43"/>
+      <c r="CZ42" s="43"/>
+      <c r="DA42" s="43"/>
+      <c r="DB42" s="43"/>
+      <c r="DC42" s="43"/>
+      <c r="DD42" s="43"/>
+      <c r="DE42" s="43"/>
+      <c r="DF42" s="43"/>
+      <c r="DG42" s="43"/>
+      <c r="DH42" s="43"/>
+      <c r="DI42" s="43"/>
+      <c r="DJ42" s="43"/>
+      <c r="DK42" s="43"/>
+      <c r="DL42" s="43"/>
+      <c r="DM42" s="43"/>
+      <c r="DN42" s="43"/>
+      <c r="DO42" s="43"/>
+      <c r="DP42" s="43"/>
+      <c r="DQ42" s="43"/>
+      <c r="DR42" s="43"/>
+      <c r="DS42" s="43"/>
+      <c r="DT42" s="43"/>
+      <c r="DU42" s="43"/>
+      <c r="DV42" s="43"/>
+      <c r="DW42" s="43"/>
+      <c r="DX42" s="43"/>
+      <c r="DY42" s="43"/>
+      <c r="DZ42" s="43"/>
+      <c r="EA42" s="43"/>
+      <c r="EB42" s="43"/>
+      <c r="EC42" s="43"/>
+      <c r="ED42" s="43"/>
+      <c r="EE42" s="43"/>
+      <c r="EF42" s="43"/>
+      <c r="EG42" s="43"/>
+      <c r="EH42" s="43"/>
+      <c r="EI42" s="43"/>
+      <c r="EJ42" s="43"/>
+      <c r="EK42" s="43"/>
+      <c r="EL42" s="43"/>
+      <c r="EM42" s="43"/>
+      <c r="EN42" s="43"/>
+      <c r="EO42" s="43"/>
+      <c r="EP42" s="43"/>
+      <c r="EQ42" s="43"/>
+      <c r="ER42" s="43"/>
+      <c r="ES42" s="43"/>
+      <c r="ET42" s="43"/>
+      <c r="EU42" s="43"/>
+      <c r="EV42" s="43"/>
+      <c r="EW42" s="43"/>
+      <c r="EX42" s="43"/>
+      <c r="EY42" s="43"/>
+      <c r="EZ42" s="43"/>
+      <c r="FA42" s="43"/>
+      <c r="FB42" s="43"/>
+      <c r="FC42" s="43"/>
+      <c r="FD42" s="43"/>
+      <c r="FE42" s="43"/>
+      <c r="FF42" s="43"/>
+      <c r="FG42" s="43"/>
+      <c r="FH42" s="43"/>
+      <c r="FI42" s="43"/>
+      <c r="FJ42" s="43"/>
+      <c r="FK42" s="43"/>
+      <c r="FL42" s="43"/>
+      <c r="FM42" s="43"/>
+      <c r="FN42" s="43"/>
+      <c r="FO42" s="43"/>
+      <c r="FP42" s="43"/>
+      <c r="FQ42" s="43"/>
+      <c r="FR42" s="43"/>
+      <c r="FS42" s="43"/>
+      <c r="FT42" s="43"/>
+      <c r="FU42" s="43"/>
+      <c r="FV42" s="43"/>
+      <c r="FW42" s="43"/>
+      <c r="FX42" s="43"/>
+      <c r="FY42" s="43"/>
+      <c r="FZ42" s="43"/>
+      <c r="GA42" s="43"/>
+      <c r="GB42" s="43"/>
+      <c r="GC42" s="43"/>
+      <c r="GD42" s="43"/>
+      <c r="GE42" s="43"/>
+      <c r="GF42" s="43"/>
+      <c r="GG42" s="43"/>
+      <c r="GH42" s="43"/>
+      <c r="GI42" s="43"/>
+      <c r="GJ42" s="43"/>
+      <c r="GK42" s="43"/>
+      <c r="GL42" s="43"/>
+      <c r="GM42" s="43"/>
+      <c r="GN42" s="43"/>
+      <c r="GO42" s="43"/>
+      <c r="GP42" s="43"/>
+      <c r="GQ42" s="43"/>
+      <c r="GR42" s="43"/>
+      <c r="GS42" s="43"/>
+      <c r="GT42" s="43"/>
+      <c r="GU42" s="43"/>
+      <c r="GV42" s="43"/>
+      <c r="GW42" s="43"/>
+      <c r="GX42" s="43"/>
+      <c r="GY42" s="43"/>
+      <c r="GZ42" s="43"/>
+      <c r="HA42" s="43"/>
+      <c r="HB42" s="43"/>
+      <c r="HC42" s="43"/>
+      <c r="HD42" s="43"/>
+      <c r="HE42" s="43"/>
+      <c r="HF42" s="43"/>
+      <c r="HG42" s="43"/>
+      <c r="HH42" s="43"/>
+      <c r="HI42" s="43"/>
+      <c r="HJ42" s="43"/>
+      <c r="HK42" s="43"/>
+      <c r="HL42" s="43"/>
+      <c r="HM42" s="43"/>
+      <c r="HN42" s="43"/>
+      <c r="HO42" s="43"/>
+      <c r="HP42" s="43"/>
+      <c r="HQ42" s="43"/>
+      <c r="HR42" s="43"/>
+      <c r="HS42" s="43"/>
+      <c r="HT42" s="43"/>
+      <c r="HU42" s="43"/>
+      <c r="HV42" s="43"/>
+      <c r="HW42" s="43"/>
+      <c r="HX42" s="43"/>
+      <c r="HY42" s="43"/>
+      <c r="HZ42" s="43"/>
+      <c r="IA42" s="43"/>
+      <c r="IB42" s="43"/>
+      <c r="IC42" s="43"/>
+      <c r="ID42" s="43"/>
+      <c r="IE42" s="43"/>
+      <c r="IF42" s="43"/>
+      <c r="IG42" s="43"/>
+      <c r="IH42" s="43"/>
+      <c r="II42" s="43"/>
+      <c r="IJ42" s="43"/>
+      <c r="IK42" s="43"/>
+      <c r="IL42" s="43"/>
+      <c r="IM42" s="43"/>
+      <c r="IN42" s="43"/>
+      <c r="IO42" s="43"/>
+      <c r="IP42" s="43"/>
+      <c r="IQ42" s="43"/>
+      <c r="IR42" s="43"/>
+      <c r="IS42" s="43"/>
+      <c r="IT42" s="43"/>
+      <c r="IU42" s="43"/>
+      <c r="IV42" s="43"/>
+    </row>
+    <row r="43" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="7"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="7"/>
+      <c r="N43" s="7"/>
+      <c r="O43" s="7"/>
+      <c r="P43" s="7"/>
+      <c r="Q43" s="7"/>
+      <c r="R43" s="43"/>
+      <c r="S43" s="43"/>
+      <c r="T43" s="43"/>
+      <c r="U43" s="43"/>
+      <c r="V43" s="43"/>
+      <c r="W43" s="43"/>
+      <c r="X43" s="43"/>
+      <c r="Y43" s="43"/>
+      <c r="Z43" s="43"/>
+      <c r="AA43" s="43"/>
+      <c r="AB43" s="43"/>
+      <c r="AC43" s="43"/>
+      <c r="AD43" s="43"/>
+      <c r="AE43" s="43"/>
+      <c r="AF43" s="43"/>
+      <c r="AG43" s="43"/>
+      <c r="AH43" s="43"/>
+      <c r="AI43" s="43"/>
+      <c r="AJ43" s="43"/>
+      <c r="AK43" s="43"/>
+      <c r="AL43" s="43"/>
+      <c r="AM43" s="43"/>
+      <c r="AN43" s="43"/>
+      <c r="AO43" s="43"/>
+      <c r="AP43" s="43"/>
+      <c r="AQ43" s="43"/>
+      <c r="AR43" s="43"/>
+      <c r="AS43" s="43"/>
+      <c r="AT43" s="43"/>
+      <c r="AU43" s="43"/>
+      <c r="AV43" s="43"/>
+      <c r="AW43" s="43"/>
+      <c r="AX43" s="43"/>
+      <c r="AY43" s="43"/>
+      <c r="AZ43" s="43"/>
+      <c r="BA43" s="43"/>
+      <c r="BB43" s="43"/>
+      <c r="BC43" s="43"/>
+      <c r="BD43" s="43"/>
+      <c r="BE43" s="43"/>
+      <c r="BF43" s="43"/>
+      <c r="BG43" s="43"/>
+      <c r="BH43" s="43"/>
+      <c r="BI43" s="43"/>
+      <c r="BJ43" s="43"/>
+      <c r="BK43" s="43"/>
+      <c r="BL43" s="43"/>
+      <c r="BM43" s="43"/>
+      <c r="BN43" s="43"/>
+      <c r="BO43" s="43"/>
+      <c r="BP43" s="43"/>
+      <c r="BQ43" s="43"/>
+      <c r="BR43" s="43"/>
+      <c r="BS43" s="43"/>
+      <c r="BT43" s="43"/>
+      <c r="BU43" s="43"/>
+      <c r="BV43" s="43"/>
+      <c r="BW43" s="43"/>
+      <c r="BX43" s="43"/>
+      <c r="BY43" s="43"/>
+      <c r="BZ43" s="43"/>
+      <c r="CA43" s="43"/>
+      <c r="CB43" s="43"/>
+      <c r="CC43" s="43"/>
+      <c r="CD43" s="43"/>
+      <c r="CE43" s="43"/>
+      <c r="CF43" s="43"/>
+      <c r="CG43" s="43"/>
+      <c r="CH43" s="43"/>
+      <c r="CI43" s="43"/>
+      <c r="CJ43" s="43"/>
+      <c r="CK43" s="43"/>
+      <c r="CL43" s="43"/>
+      <c r="CM43" s="43"/>
+      <c r="CN43" s="43"/>
+      <c r="CO43" s="43"/>
+      <c r="CP43" s="43"/>
+      <c r="CQ43" s="43"/>
+      <c r="CR43" s="43"/>
+      <c r="CS43" s="43"/>
+      <c r="CT43" s="43"/>
+      <c r="CU43" s="43"/>
+      <c r="CV43" s="43"/>
+      <c r="CW43" s="43"/>
+      <c r="CX43" s="43"/>
+      <c r="CY43" s="43"/>
+      <c r="CZ43" s="43"/>
+      <c r="DA43" s="43"/>
+      <c r="DB43" s="43"/>
+      <c r="DC43" s="43"/>
+      <c r="DD43" s="43"/>
+      <c r="DE43" s="43"/>
+      <c r="DF43" s="43"/>
+      <c r="DG43" s="43"/>
+      <c r="DH43" s="43"/>
+      <c r="DI43" s="43"/>
+      <c r="DJ43" s="43"/>
+      <c r="DK43" s="43"/>
+      <c r="DL43" s="43"/>
+      <c r="DM43" s="43"/>
+      <c r="DN43" s="43"/>
+      <c r="DO43" s="43"/>
+      <c r="DP43" s="43"/>
+      <c r="DQ43" s="43"/>
+      <c r="DR43" s="43"/>
+      <c r="DS43" s="43"/>
+      <c r="DT43" s="43"/>
+      <c r="DU43" s="43"/>
+      <c r="DV43" s="43"/>
+      <c r="DW43" s="43"/>
+      <c r="DX43" s="43"/>
+      <c r="DY43" s="43"/>
+      <c r="DZ43" s="43"/>
+      <c r="EA43" s="43"/>
+      <c r="EB43" s="43"/>
+      <c r="EC43" s="43"/>
+      <c r="ED43" s="43"/>
+      <c r="EE43" s="43"/>
+      <c r="EF43" s="43"/>
+      <c r="EG43" s="43"/>
+      <c r="EH43" s="43"/>
+      <c r="EI43" s="43"/>
+      <c r="EJ43" s="43"/>
+      <c r="EK43" s="43"/>
+      <c r="EL43" s="43"/>
+      <c r="EM43" s="43"/>
+      <c r="EN43" s="43"/>
+      <c r="EO43" s="43"/>
+      <c r="EP43" s="43"/>
+      <c r="EQ43" s="43"/>
+      <c r="ER43" s="43"/>
+      <c r="ES43" s="43"/>
+      <c r="ET43" s="43"/>
+      <c r="EU43" s="43"/>
+      <c r="EV43" s="43"/>
+      <c r="EW43" s="43"/>
+      <c r="EX43" s="43"/>
+      <c r="EY43" s="43"/>
+      <c r="EZ43" s="43"/>
+      <c r="FA43" s="43"/>
+      <c r="FB43" s="43"/>
+      <c r="FC43" s="43"/>
+      <c r="FD43" s="43"/>
+      <c r="FE43" s="43"/>
+      <c r="FF43" s="43"/>
+      <c r="FG43" s="43"/>
+      <c r="FH43" s="43"/>
+      <c r="FI43" s="43"/>
+      <c r="FJ43" s="43"/>
+      <c r="FK43" s="43"/>
+      <c r="FL43" s="43"/>
+      <c r="FM43" s="43"/>
+      <c r="FN43" s="43"/>
+      <c r="FO43" s="43"/>
+      <c r="FP43" s="43"/>
+      <c r="FQ43" s="43"/>
+      <c r="FR43" s="43"/>
+      <c r="FS43" s="43"/>
+      <c r="FT43" s="43"/>
+      <c r="FU43" s="43"/>
+      <c r="FV43" s="43"/>
+      <c r="FW43" s="43"/>
+      <c r="FX43" s="43"/>
+      <c r="FY43" s="43"/>
+      <c r="FZ43" s="43"/>
+      <c r="GA43" s="43"/>
+      <c r="GB43" s="43"/>
+      <c r="GC43" s="43"/>
+      <c r="GD43" s="43"/>
+      <c r="GE43" s="43"/>
+      <c r="GF43" s="43"/>
+      <c r="GG43" s="43"/>
+      <c r="GH43" s="43"/>
+      <c r="GI43" s="43"/>
+      <c r="GJ43" s="43"/>
+      <c r="GK43" s="43"/>
+      <c r="GL43" s="43"/>
+      <c r="GM43" s="43"/>
+      <c r="GN43" s="43"/>
+      <c r="GO43" s="43"/>
+      <c r="GP43" s="43"/>
+      <c r="GQ43" s="43"/>
+      <c r="GR43" s="43"/>
+      <c r="GS43" s="43"/>
+      <c r="GT43" s="43"/>
+      <c r="GU43" s="43"/>
+      <c r="GV43" s="43"/>
+      <c r="GW43" s="43"/>
+      <c r="GX43" s="43"/>
+      <c r="GY43" s="43"/>
+      <c r="GZ43" s="43"/>
+      <c r="HA43" s="43"/>
+      <c r="HB43" s="43"/>
+      <c r="HC43" s="43"/>
+      <c r="HD43" s="43"/>
+      <c r="HE43" s="43"/>
+      <c r="HF43" s="43"/>
+      <c r="HG43" s="43"/>
+      <c r="HH43" s="43"/>
+      <c r="HI43" s="43"/>
+      <c r="HJ43" s="43"/>
+      <c r="HK43" s="43"/>
+      <c r="HL43" s="43"/>
+      <c r="HM43" s="43"/>
+      <c r="HN43" s="43"/>
+      <c r="HO43" s="43"/>
+      <c r="HP43" s="43"/>
+      <c r="HQ43" s="43"/>
+      <c r="HR43" s="43"/>
+      <c r="HS43" s="43"/>
+      <c r="HT43" s="43"/>
+      <c r="HU43" s="43"/>
+      <c r="HV43" s="43"/>
+      <c r="HW43" s="43"/>
+      <c r="HX43" s="43"/>
+      <c r="HY43" s="43"/>
+      <c r="HZ43" s="43"/>
+      <c r="IA43" s="43"/>
+      <c r="IB43" s="43"/>
+      <c r="IC43" s="43"/>
+      <c r="ID43" s="43"/>
+      <c r="IE43" s="43"/>
+      <c r="IF43" s="43"/>
+      <c r="IG43" s="43"/>
+      <c r="IH43" s="43"/>
+      <c r="II43" s="43"/>
+      <c r="IJ43" s="43"/>
+      <c r="IK43" s="43"/>
+      <c r="IL43" s="43"/>
+      <c r="IM43" s="43"/>
+      <c r="IN43" s="43"/>
+      <c r="IO43" s="43"/>
+      <c r="IP43" s="43"/>
+      <c r="IQ43" s="43"/>
+      <c r="IR43" s="43"/>
+      <c r="IS43" s="43"/>
+      <c r="IT43" s="43"/>
+      <c r="IU43" s="43"/>
+      <c r="IV43" s="43"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -14437,7 +15012,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="D1" workbookViewId="0">
@@ -15365,7 +15940,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -15696,11 +16271,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:N27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -16407,22 +16982,22 @@
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="8" t="s">
-        <v>395</v>
+        <v>376</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>157</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>156</v>
+        <v>415</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>156</v>
+        <v>415</v>
       </c>
       <c r="G22" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>66</v>
+        <v>418</v>
       </c>
       <c r="I22" s="6">
         <v>1</v>
@@ -16433,22 +17008,22 @@
       <c r="M22" s="7"/>
       <c r="N22" s="7"/>
     </row>
-    <row r="23" spans="1:14" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:14" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10">
         <v>42736</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="8" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="E23" s="58" t="s">
-        <v>364</v>
-      </c>
-      <c r="F23" s="58" t="s">
-        <v>361</v>
+      <c r="E23" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>156</v>
       </c>
       <c r="G23" s="6">
         <v>1</v>
@@ -16460,9 +17035,7 @@
         <v>1</v>
       </c>
       <c r="J23" s="7"/>
-      <c r="K23" s="60" t="s">
-        <v>403</v>
-      </c>
+      <c r="K23" s="7"/>
       <c r="L23" s="7"/>
       <c r="M23" s="7"/>
       <c r="N23" s="7"/>
@@ -16488,20 +17061,54 @@
         <v>1</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>339</v>
+        <v>66</v>
       </c>
       <c r="I24" s="6">
         <v>1</v>
       </c>
-      <c r="J24" s="60" t="s">
-        <v>407</v>
-      </c>
-      <c r="K24" s="60"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="60" t="s">
+        <v>403</v>
+      </c>
       <c r="L24" s="7"/>
       <c r="M24" s="7"/>
       <c r="N24" s="7"/>
     </row>
-    <row r="27" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="25" spans="1:14" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B25" s="10"/>
+      <c r="C25" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E25" s="58" t="s">
+        <v>364</v>
+      </c>
+      <c r="F25" s="58" t="s">
+        <v>361</v>
+      </c>
+      <c r="G25" s="6">
+        <v>1</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="I25" s="6">
+        <v>1</v>
+      </c>
+      <c r="J25" s="60" t="s">
+        <v>407</v>
+      </c>
+      <c r="K25" s="60"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+    </row>
+    <row r="28" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -16512,7 +17119,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -16865,10 +17472,10 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="L1" workbookViewId="0">
       <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
@@ -17562,7 +18169,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB42"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">

</xml_diff>

<commit_message>
RDM-4184 Update func tests and spreadsheet to reflect removing of the… (#637)
* RDM-4184 Update func tests and spreadsheet to reflect removing of the fixed History tab.

* Update conditionalLogic.feature
</commit_message>
<xml_diff>
--- a/test/resources/definitionsFiles/fe-automation-definition-v03.xlsx
+++ b/test/resources/definitionsFiles/fe-automation-definition-v03.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dev/Documents/Definition Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrzejfolga/src/ccd/temp/ccd-case-management-web/test/resources/definitionsFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C03B15-2E2B-B642-8670-12D7B70880B4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" firstSheet="7" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -33,7 +32,7 @@
     <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId18"/>
     <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -46,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1704" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1718" uniqueCount="419">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1365,17 +1364,29 @@
   </si>
   <si>
     <t>Case Reference</t>
+  </si>
+  <si>
+    <t>history</t>
+  </si>
+  <si>
+    <t>Case History</t>
+  </si>
+  <si>
+    <t>CaseHistoryViewer</t>
+  </si>
+  <si>
+    <t>CaseHistory</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;DD/&quot;mm&quot;/YYYY&quot;"/>
     <numFmt numFmtId="165" formatCode="&quot;D/&quot;m&quot;/YY&quot;"/>
   </numFmts>
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -1556,6 +1567,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1663,12 +1681,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1753,11 +1773,15 @@
     <xf numFmtId="164" fontId="29" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="29" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="23" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="23" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7"/>
@@ -2914,7 +2938,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3098,7 +3122,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3596,7 +3620,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3857,7 +3881,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -4067,7 +4091,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -4355,7 +4379,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -4500,7 +4524,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-0D00-000003000000}"/>
+    <hyperlink ref="C4" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -4511,7 +4535,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -4707,11 +4731,11 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:K41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:XFD38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5571,11 +5595,11 @@
         <v>42736</v>
       </c>
       <c r="B38" s="10"/>
-      <c r="C38" s="8" t="s">
-        <v>395</v>
+      <c r="C38" s="58" t="s">
+        <v>376</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>66</v>
+        <v>418</v>
       </c>
       <c r="E38" t="s">
         <v>271</v>
@@ -5595,7 +5619,7 @@
       </c>
       <c r="B39" s="10"/>
       <c r="C39" s="8" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>66</v>
@@ -5620,8 +5644,8 @@
       <c r="C40" s="8" t="s">
         <v>400</v>
       </c>
-      <c r="D40" s="58" t="s">
-        <v>336</v>
+      <c r="D40" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="E40" t="s">
         <v>271</v>
@@ -5644,7 +5668,7 @@
         <v>400</v>
       </c>
       <c r="D41" s="58" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E41" t="s">
         <v>271</v>
@@ -5657,6 +5681,29 @@
       <c r="I41" s="7"/>
       <c r="J41" s="7"/>
       <c r="K41" s="7"/>
+    </row>
+    <row r="42" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B42" s="10"/>
+      <c r="C42" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="D42" s="58" t="s">
+        <v>339</v>
+      </c>
+      <c r="E42" t="s">
+        <v>271</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="G42" s="8"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
@@ -5668,7 +5715,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5784,7 +5831,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
@@ -6182,7 +6229,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -6560,7 +6607,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
@@ -6874,7 +6921,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G4" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="G4" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -6885,11 +6932,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:IV41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV43"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+    <sheetView showGridLines="0" topLeftCell="C3" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -13349,34 +13396,32 @@
       <c r="A38" s="10">
         <v>42736</v>
       </c>
-      <c r="B38" s="10"/>
-      <c r="C38" s="8" t="s">
-        <v>395</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="F38" s="7"/>
-      <c r="G38" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7" t="s">
-        <v>398</v>
-      </c>
-      <c r="J38" s="8" t="s">
+      <c r="B38" s="74"/>
+      <c r="C38" s="58" t="s">
+        <v>376</v>
+      </c>
+      <c r="D38" s="73" t="s">
+        <v>418</v>
+      </c>
+      <c r="E38" s="73" t="s">
+        <v>416</v>
+      </c>
+      <c r="F38" s="75"/>
+      <c r="G38" s="73" t="s">
+        <v>417</v>
+      </c>
+      <c r="H38" s="75"/>
+      <c r="I38" s="75"/>
+      <c r="J38" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="K38" s="7"/>
-      <c r="L38" s="7"/>
-      <c r="M38" s="7"/>
-      <c r="N38" s="7"/>
-      <c r="O38" s="7"/>
-      <c r="P38" s="7"/>
-      <c r="Q38" s="7"/>
+      <c r="K38" s="75"/>
+      <c r="L38" s="75"/>
+      <c r="M38" s="75"/>
+      <c r="N38" s="75"/>
+      <c r="O38" s="75"/>
+      <c r="P38" s="75"/>
+      <c r="Q38" s="75"/>
       <c r="R38" s="43"/>
       <c r="S38" s="43"/>
       <c r="T38" s="43"/>
@@ -13623,7 +13668,7 @@
       </c>
       <c r="B39" s="10"/>
       <c r="C39" s="8" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>66</v>
@@ -13636,7 +13681,9 @@
         <v>48</v>
       </c>
       <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
+      <c r="I39" s="7" t="s">
+        <v>398</v>
+      </c>
       <c r="J39" s="8" t="s">
         <v>27</v>
       </c>
@@ -13895,11 +13942,11 @@
       <c r="C40" s="8" t="s">
         <v>400</v>
       </c>
-      <c r="D40" s="58" t="s">
-        <v>336</v>
-      </c>
-      <c r="E40" s="58" t="s">
-        <v>334</v>
+      <c r="D40" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>67</v>
       </c>
       <c r="F40" s="7"/>
       <c r="G40" s="8" t="s">
@@ -14166,10 +14213,10 @@
         <v>400</v>
       </c>
       <c r="D41" s="58" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E41" s="58" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="F41" s="7"/>
       <c r="G41" s="8" t="s">
@@ -14427,6 +14474,534 @@
       <c r="IU41" s="43"/>
       <c r="IV41" s="43"/>
     </row>
+    <row r="42" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B42" s="10"/>
+      <c r="C42" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="D42" s="58" t="s">
+        <v>339</v>
+      </c>
+      <c r="E42" s="58" t="s">
+        <v>343</v>
+      </c>
+      <c r="F42" s="7"/>
+      <c r="G42" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K42" s="7"/>
+      <c r="L42" s="7"/>
+      <c r="M42" s="7"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="7"/>
+      <c r="P42" s="7"/>
+      <c r="Q42" s="7"/>
+      <c r="R42" s="43"/>
+      <c r="S42" s="43"/>
+      <c r="T42" s="43"/>
+      <c r="U42" s="43"/>
+      <c r="V42" s="43"/>
+      <c r="W42" s="43"/>
+      <c r="X42" s="43"/>
+      <c r="Y42" s="43"/>
+      <c r="Z42" s="43"/>
+      <c r="AA42" s="43"/>
+      <c r="AB42" s="43"/>
+      <c r="AC42" s="43"/>
+      <c r="AD42" s="43"/>
+      <c r="AE42" s="43"/>
+      <c r="AF42" s="43"/>
+      <c r="AG42" s="43"/>
+      <c r="AH42" s="43"/>
+      <c r="AI42" s="43"/>
+      <c r="AJ42" s="43"/>
+      <c r="AK42" s="43"/>
+      <c r="AL42" s="43"/>
+      <c r="AM42" s="43"/>
+      <c r="AN42" s="43"/>
+      <c r="AO42" s="43"/>
+      <c r="AP42" s="43"/>
+      <c r="AQ42" s="43"/>
+      <c r="AR42" s="43"/>
+      <c r="AS42" s="43"/>
+      <c r="AT42" s="43"/>
+      <c r="AU42" s="43"/>
+      <c r="AV42" s="43"/>
+      <c r="AW42" s="43"/>
+      <c r="AX42" s="43"/>
+      <c r="AY42" s="43"/>
+      <c r="AZ42" s="43"/>
+      <c r="BA42" s="43"/>
+      <c r="BB42" s="43"/>
+      <c r="BC42" s="43"/>
+      <c r="BD42" s="43"/>
+      <c r="BE42" s="43"/>
+      <c r="BF42" s="43"/>
+      <c r="BG42" s="43"/>
+      <c r="BH42" s="43"/>
+      <c r="BI42" s="43"/>
+      <c r="BJ42" s="43"/>
+      <c r="BK42" s="43"/>
+      <c r="BL42" s="43"/>
+      <c r="BM42" s="43"/>
+      <c r="BN42" s="43"/>
+      <c r="BO42" s="43"/>
+      <c r="BP42" s="43"/>
+      <c r="BQ42" s="43"/>
+      <c r="BR42" s="43"/>
+      <c r="BS42" s="43"/>
+      <c r="BT42" s="43"/>
+      <c r="BU42" s="43"/>
+      <c r="BV42" s="43"/>
+      <c r="BW42" s="43"/>
+      <c r="BX42" s="43"/>
+      <c r="BY42" s="43"/>
+      <c r="BZ42" s="43"/>
+      <c r="CA42" s="43"/>
+      <c r="CB42" s="43"/>
+      <c r="CC42" s="43"/>
+      <c r="CD42" s="43"/>
+      <c r="CE42" s="43"/>
+      <c r="CF42" s="43"/>
+      <c r="CG42" s="43"/>
+      <c r="CH42" s="43"/>
+      <c r="CI42" s="43"/>
+      <c r="CJ42" s="43"/>
+      <c r="CK42" s="43"/>
+      <c r="CL42" s="43"/>
+      <c r="CM42" s="43"/>
+      <c r="CN42" s="43"/>
+      <c r="CO42" s="43"/>
+      <c r="CP42" s="43"/>
+      <c r="CQ42" s="43"/>
+      <c r="CR42" s="43"/>
+      <c r="CS42" s="43"/>
+      <c r="CT42" s="43"/>
+      <c r="CU42" s="43"/>
+      <c r="CV42" s="43"/>
+      <c r="CW42" s="43"/>
+      <c r="CX42" s="43"/>
+      <c r="CY42" s="43"/>
+      <c r="CZ42" s="43"/>
+      <c r="DA42" s="43"/>
+      <c r="DB42" s="43"/>
+      <c r="DC42" s="43"/>
+      <c r="DD42" s="43"/>
+      <c r="DE42" s="43"/>
+      <c r="DF42" s="43"/>
+      <c r="DG42" s="43"/>
+      <c r="DH42" s="43"/>
+      <c r="DI42" s="43"/>
+      <c r="DJ42" s="43"/>
+      <c r="DK42" s="43"/>
+      <c r="DL42" s="43"/>
+      <c r="DM42" s="43"/>
+      <c r="DN42" s="43"/>
+      <c r="DO42" s="43"/>
+      <c r="DP42" s="43"/>
+      <c r="DQ42" s="43"/>
+      <c r="DR42" s="43"/>
+      <c r="DS42" s="43"/>
+      <c r="DT42" s="43"/>
+      <c r="DU42" s="43"/>
+      <c r="DV42" s="43"/>
+      <c r="DW42" s="43"/>
+      <c r="DX42" s="43"/>
+      <c r="DY42" s="43"/>
+      <c r="DZ42" s="43"/>
+      <c r="EA42" s="43"/>
+      <c r="EB42" s="43"/>
+      <c r="EC42" s="43"/>
+      <c r="ED42" s="43"/>
+      <c r="EE42" s="43"/>
+      <c r="EF42" s="43"/>
+      <c r="EG42" s="43"/>
+      <c r="EH42" s="43"/>
+      <c r="EI42" s="43"/>
+      <c r="EJ42" s="43"/>
+      <c r="EK42" s="43"/>
+      <c r="EL42" s="43"/>
+      <c r="EM42" s="43"/>
+      <c r="EN42" s="43"/>
+      <c r="EO42" s="43"/>
+      <c r="EP42" s="43"/>
+      <c r="EQ42" s="43"/>
+      <c r="ER42" s="43"/>
+      <c r="ES42" s="43"/>
+      <c r="ET42" s="43"/>
+      <c r="EU42" s="43"/>
+      <c r="EV42" s="43"/>
+      <c r="EW42" s="43"/>
+      <c r="EX42" s="43"/>
+      <c r="EY42" s="43"/>
+      <c r="EZ42" s="43"/>
+      <c r="FA42" s="43"/>
+      <c r="FB42" s="43"/>
+      <c r="FC42" s="43"/>
+      <c r="FD42" s="43"/>
+      <c r="FE42" s="43"/>
+      <c r="FF42" s="43"/>
+      <c r="FG42" s="43"/>
+      <c r="FH42" s="43"/>
+      <c r="FI42" s="43"/>
+      <c r="FJ42" s="43"/>
+      <c r="FK42" s="43"/>
+      <c r="FL42" s="43"/>
+      <c r="FM42" s="43"/>
+      <c r="FN42" s="43"/>
+      <c r="FO42" s="43"/>
+      <c r="FP42" s="43"/>
+      <c r="FQ42" s="43"/>
+      <c r="FR42" s="43"/>
+      <c r="FS42" s="43"/>
+      <c r="FT42" s="43"/>
+      <c r="FU42" s="43"/>
+      <c r="FV42" s="43"/>
+      <c r="FW42" s="43"/>
+      <c r="FX42" s="43"/>
+      <c r="FY42" s="43"/>
+      <c r="FZ42" s="43"/>
+      <c r="GA42" s="43"/>
+      <c r="GB42" s="43"/>
+      <c r="GC42" s="43"/>
+      <c r="GD42" s="43"/>
+      <c r="GE42" s="43"/>
+      <c r="GF42" s="43"/>
+      <c r="GG42" s="43"/>
+      <c r="GH42" s="43"/>
+      <c r="GI42" s="43"/>
+      <c r="GJ42" s="43"/>
+      <c r="GK42" s="43"/>
+      <c r="GL42" s="43"/>
+      <c r="GM42" s="43"/>
+      <c r="GN42" s="43"/>
+      <c r="GO42" s="43"/>
+      <c r="GP42" s="43"/>
+      <c r="GQ42" s="43"/>
+      <c r="GR42" s="43"/>
+      <c r="GS42" s="43"/>
+      <c r="GT42" s="43"/>
+      <c r="GU42" s="43"/>
+      <c r="GV42" s="43"/>
+      <c r="GW42" s="43"/>
+      <c r="GX42" s="43"/>
+      <c r="GY42" s="43"/>
+      <c r="GZ42" s="43"/>
+      <c r="HA42" s="43"/>
+      <c r="HB42" s="43"/>
+      <c r="HC42" s="43"/>
+      <c r="HD42" s="43"/>
+      <c r="HE42" s="43"/>
+      <c r="HF42" s="43"/>
+      <c r="HG42" s="43"/>
+      <c r="HH42" s="43"/>
+      <c r="HI42" s="43"/>
+      <c r="HJ42" s="43"/>
+      <c r="HK42" s="43"/>
+      <c r="HL42" s="43"/>
+      <c r="HM42" s="43"/>
+      <c r="HN42" s="43"/>
+      <c r="HO42" s="43"/>
+      <c r="HP42" s="43"/>
+      <c r="HQ42" s="43"/>
+      <c r="HR42" s="43"/>
+      <c r="HS42" s="43"/>
+      <c r="HT42" s="43"/>
+      <c r="HU42" s="43"/>
+      <c r="HV42" s="43"/>
+      <c r="HW42" s="43"/>
+      <c r="HX42" s="43"/>
+      <c r="HY42" s="43"/>
+      <c r="HZ42" s="43"/>
+      <c r="IA42" s="43"/>
+      <c r="IB42" s="43"/>
+      <c r="IC42" s="43"/>
+      <c r="ID42" s="43"/>
+      <c r="IE42" s="43"/>
+      <c r="IF42" s="43"/>
+      <c r="IG42" s="43"/>
+      <c r="IH42" s="43"/>
+      <c r="II42" s="43"/>
+      <c r="IJ42" s="43"/>
+      <c r="IK42" s="43"/>
+      <c r="IL42" s="43"/>
+      <c r="IM42" s="43"/>
+      <c r="IN42" s="43"/>
+      <c r="IO42" s="43"/>
+      <c r="IP42" s="43"/>
+      <c r="IQ42" s="43"/>
+      <c r="IR42" s="43"/>
+      <c r="IS42" s="43"/>
+      <c r="IT42" s="43"/>
+      <c r="IU42" s="43"/>
+      <c r="IV42" s="43"/>
+    </row>
+    <row r="43" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="7"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="7"/>
+      <c r="N43" s="7"/>
+      <c r="O43" s="7"/>
+      <c r="P43" s="7"/>
+      <c r="Q43" s="7"/>
+      <c r="R43" s="43"/>
+      <c r="S43" s="43"/>
+      <c r="T43" s="43"/>
+      <c r="U43" s="43"/>
+      <c r="V43" s="43"/>
+      <c r="W43" s="43"/>
+      <c r="X43" s="43"/>
+      <c r="Y43" s="43"/>
+      <c r="Z43" s="43"/>
+      <c r="AA43" s="43"/>
+      <c r="AB43" s="43"/>
+      <c r="AC43" s="43"/>
+      <c r="AD43" s="43"/>
+      <c r="AE43" s="43"/>
+      <c r="AF43" s="43"/>
+      <c r="AG43" s="43"/>
+      <c r="AH43" s="43"/>
+      <c r="AI43" s="43"/>
+      <c r="AJ43" s="43"/>
+      <c r="AK43" s="43"/>
+      <c r="AL43" s="43"/>
+      <c r="AM43" s="43"/>
+      <c r="AN43" s="43"/>
+      <c r="AO43" s="43"/>
+      <c r="AP43" s="43"/>
+      <c r="AQ43" s="43"/>
+      <c r="AR43" s="43"/>
+      <c r="AS43" s="43"/>
+      <c r="AT43" s="43"/>
+      <c r="AU43" s="43"/>
+      <c r="AV43" s="43"/>
+      <c r="AW43" s="43"/>
+      <c r="AX43" s="43"/>
+      <c r="AY43" s="43"/>
+      <c r="AZ43" s="43"/>
+      <c r="BA43" s="43"/>
+      <c r="BB43" s="43"/>
+      <c r="BC43" s="43"/>
+      <c r="BD43" s="43"/>
+      <c r="BE43" s="43"/>
+      <c r="BF43" s="43"/>
+      <c r="BG43" s="43"/>
+      <c r="BH43" s="43"/>
+      <c r="BI43" s="43"/>
+      <c r="BJ43" s="43"/>
+      <c r="BK43" s="43"/>
+      <c r="BL43" s="43"/>
+      <c r="BM43" s="43"/>
+      <c r="BN43" s="43"/>
+      <c r="BO43" s="43"/>
+      <c r="BP43" s="43"/>
+      <c r="BQ43" s="43"/>
+      <c r="BR43" s="43"/>
+      <c r="BS43" s="43"/>
+      <c r="BT43" s="43"/>
+      <c r="BU43" s="43"/>
+      <c r="BV43" s="43"/>
+      <c r="BW43" s="43"/>
+      <c r="BX43" s="43"/>
+      <c r="BY43" s="43"/>
+      <c r="BZ43" s="43"/>
+      <c r="CA43" s="43"/>
+      <c r="CB43" s="43"/>
+      <c r="CC43" s="43"/>
+      <c r="CD43" s="43"/>
+      <c r="CE43" s="43"/>
+      <c r="CF43" s="43"/>
+      <c r="CG43" s="43"/>
+      <c r="CH43" s="43"/>
+      <c r="CI43" s="43"/>
+      <c r="CJ43" s="43"/>
+      <c r="CK43" s="43"/>
+      <c r="CL43" s="43"/>
+      <c r="CM43" s="43"/>
+      <c r="CN43" s="43"/>
+      <c r="CO43" s="43"/>
+      <c r="CP43" s="43"/>
+      <c r="CQ43" s="43"/>
+      <c r="CR43" s="43"/>
+      <c r="CS43" s="43"/>
+      <c r="CT43" s="43"/>
+      <c r="CU43" s="43"/>
+      <c r="CV43" s="43"/>
+      <c r="CW43" s="43"/>
+      <c r="CX43" s="43"/>
+      <c r="CY43" s="43"/>
+      <c r="CZ43" s="43"/>
+      <c r="DA43" s="43"/>
+      <c r="DB43" s="43"/>
+      <c r="DC43" s="43"/>
+      <c r="DD43" s="43"/>
+      <c r="DE43" s="43"/>
+      <c r="DF43" s="43"/>
+      <c r="DG43" s="43"/>
+      <c r="DH43" s="43"/>
+      <c r="DI43" s="43"/>
+      <c r="DJ43" s="43"/>
+      <c r="DK43" s="43"/>
+      <c r="DL43" s="43"/>
+      <c r="DM43" s="43"/>
+      <c r="DN43" s="43"/>
+      <c r="DO43" s="43"/>
+      <c r="DP43" s="43"/>
+      <c r="DQ43" s="43"/>
+      <c r="DR43" s="43"/>
+      <c r="DS43" s="43"/>
+      <c r="DT43" s="43"/>
+      <c r="DU43" s="43"/>
+      <c r="DV43" s="43"/>
+      <c r="DW43" s="43"/>
+      <c r="DX43" s="43"/>
+      <c r="DY43" s="43"/>
+      <c r="DZ43" s="43"/>
+      <c r="EA43" s="43"/>
+      <c r="EB43" s="43"/>
+      <c r="EC43" s="43"/>
+      <c r="ED43" s="43"/>
+      <c r="EE43" s="43"/>
+      <c r="EF43" s="43"/>
+      <c r="EG43" s="43"/>
+      <c r="EH43" s="43"/>
+      <c r="EI43" s="43"/>
+      <c r="EJ43" s="43"/>
+      <c r="EK43" s="43"/>
+      <c r="EL43" s="43"/>
+      <c r="EM43" s="43"/>
+      <c r="EN43" s="43"/>
+      <c r="EO43" s="43"/>
+      <c r="EP43" s="43"/>
+      <c r="EQ43" s="43"/>
+      <c r="ER43" s="43"/>
+      <c r="ES43" s="43"/>
+      <c r="ET43" s="43"/>
+      <c r="EU43" s="43"/>
+      <c r="EV43" s="43"/>
+      <c r="EW43" s="43"/>
+      <c r="EX43" s="43"/>
+      <c r="EY43" s="43"/>
+      <c r="EZ43" s="43"/>
+      <c r="FA43" s="43"/>
+      <c r="FB43" s="43"/>
+      <c r="FC43" s="43"/>
+      <c r="FD43" s="43"/>
+      <c r="FE43" s="43"/>
+      <c r="FF43" s="43"/>
+      <c r="FG43" s="43"/>
+      <c r="FH43" s="43"/>
+      <c r="FI43" s="43"/>
+      <c r="FJ43" s="43"/>
+      <c r="FK43" s="43"/>
+      <c r="FL43" s="43"/>
+      <c r="FM43" s="43"/>
+      <c r="FN43" s="43"/>
+      <c r="FO43" s="43"/>
+      <c r="FP43" s="43"/>
+      <c r="FQ43" s="43"/>
+      <c r="FR43" s="43"/>
+      <c r="FS43" s="43"/>
+      <c r="FT43" s="43"/>
+      <c r="FU43" s="43"/>
+      <c r="FV43" s="43"/>
+      <c r="FW43" s="43"/>
+      <c r="FX43" s="43"/>
+      <c r="FY43" s="43"/>
+      <c r="FZ43" s="43"/>
+      <c r="GA43" s="43"/>
+      <c r="GB43" s="43"/>
+      <c r="GC43" s="43"/>
+      <c r="GD43" s="43"/>
+      <c r="GE43" s="43"/>
+      <c r="GF43" s="43"/>
+      <c r="GG43" s="43"/>
+      <c r="GH43" s="43"/>
+      <c r="GI43" s="43"/>
+      <c r="GJ43" s="43"/>
+      <c r="GK43" s="43"/>
+      <c r="GL43" s="43"/>
+      <c r="GM43" s="43"/>
+      <c r="GN43" s="43"/>
+      <c r="GO43" s="43"/>
+      <c r="GP43" s="43"/>
+      <c r="GQ43" s="43"/>
+      <c r="GR43" s="43"/>
+      <c r="GS43" s="43"/>
+      <c r="GT43" s="43"/>
+      <c r="GU43" s="43"/>
+      <c r="GV43" s="43"/>
+      <c r="GW43" s="43"/>
+      <c r="GX43" s="43"/>
+      <c r="GY43" s="43"/>
+      <c r="GZ43" s="43"/>
+      <c r="HA43" s="43"/>
+      <c r="HB43" s="43"/>
+      <c r="HC43" s="43"/>
+      <c r="HD43" s="43"/>
+      <c r="HE43" s="43"/>
+      <c r="HF43" s="43"/>
+      <c r="HG43" s="43"/>
+      <c r="HH43" s="43"/>
+      <c r="HI43" s="43"/>
+      <c r="HJ43" s="43"/>
+      <c r="HK43" s="43"/>
+      <c r="HL43" s="43"/>
+      <c r="HM43" s="43"/>
+      <c r="HN43" s="43"/>
+      <c r="HO43" s="43"/>
+      <c r="HP43" s="43"/>
+      <c r="HQ43" s="43"/>
+      <c r="HR43" s="43"/>
+      <c r="HS43" s="43"/>
+      <c r="HT43" s="43"/>
+      <c r="HU43" s="43"/>
+      <c r="HV43" s="43"/>
+      <c r="HW43" s="43"/>
+      <c r="HX43" s="43"/>
+      <c r="HY43" s="43"/>
+      <c r="HZ43" s="43"/>
+      <c r="IA43" s="43"/>
+      <c r="IB43" s="43"/>
+      <c r="IC43" s="43"/>
+      <c r="ID43" s="43"/>
+      <c r="IE43" s="43"/>
+      <c r="IF43" s="43"/>
+      <c r="IG43" s="43"/>
+      <c r="IH43" s="43"/>
+      <c r="II43" s="43"/>
+      <c r="IJ43" s="43"/>
+      <c r="IK43" s="43"/>
+      <c r="IL43" s="43"/>
+      <c r="IM43" s="43"/>
+      <c r="IN43" s="43"/>
+      <c r="IO43" s="43"/>
+      <c r="IP43" s="43"/>
+      <c r="IQ43" s="43"/>
+      <c r="IR43" s="43"/>
+      <c r="IS43" s="43"/>
+      <c r="IT43" s="43"/>
+      <c r="IU43" s="43"/>
+      <c r="IV43" s="43"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -14437,7 +15012,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="D1" workbookViewId="0">
@@ -15365,7 +15940,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -15696,11 +16271,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:N27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -16407,22 +16982,22 @@
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="8" t="s">
-        <v>395</v>
+        <v>376</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>157</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>156</v>
+        <v>415</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>156</v>
+        <v>415</v>
       </c>
       <c r="G22" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>66</v>
+        <v>418</v>
       </c>
       <c r="I22" s="6">
         <v>1</v>
@@ -16433,22 +17008,22 @@
       <c r="M22" s="7"/>
       <c r="N22" s="7"/>
     </row>
-    <row r="23" spans="1:14" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:14" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10">
         <v>42736</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="8" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="E23" s="58" t="s">
-        <v>364</v>
-      </c>
-      <c r="F23" s="58" t="s">
-        <v>361</v>
+      <c r="E23" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>156</v>
       </c>
       <c r="G23" s="6">
         <v>1</v>
@@ -16460,9 +17035,7 @@
         <v>1</v>
       </c>
       <c r="J23" s="7"/>
-      <c r="K23" s="60" t="s">
-        <v>403</v>
-      </c>
+      <c r="K23" s="7"/>
       <c r="L23" s="7"/>
       <c r="M23" s="7"/>
       <c r="N23" s="7"/>
@@ -16488,20 +17061,54 @@
         <v>1</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>339</v>
+        <v>66</v>
       </c>
       <c r="I24" s="6">
         <v>1</v>
       </c>
-      <c r="J24" s="60" t="s">
-        <v>407</v>
-      </c>
-      <c r="K24" s="60"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="60" t="s">
+        <v>403</v>
+      </c>
       <c r="L24" s="7"/>
       <c r="M24" s="7"/>
       <c r="N24" s="7"/>
     </row>
-    <row r="27" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="25" spans="1:14" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B25" s="10"/>
+      <c r="C25" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E25" s="58" t="s">
+        <v>364</v>
+      </c>
+      <c r="F25" s="58" t="s">
+        <v>361</v>
+      </c>
+      <c r="G25" s="6">
+        <v>1</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="I25" s="6">
+        <v>1</v>
+      </c>
+      <c r="J25" s="60" t="s">
+        <v>407</v>
+      </c>
+      <c r="K25" s="60"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+    </row>
+    <row r="28" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -16512,7 +17119,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -16865,10 +17472,10 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="L1" workbookViewId="0">
       <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
@@ -17562,7 +18169,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB42"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">

</xml_diff>